<commit_message>
anik fixed asset schedule
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/depreciation.xlsx
+++ b/afar_project/csv_path/excel_files/depreciation.xlsx
@@ -637,7 +637,9 @@
       <c r="M2" t="n">
         <v>56862</v>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
       <c r="O2" t="n">
         <v>7</v>
       </c>
@@ -753,7 +755,9 @@
       <c r="M3" t="n">
         <v>22253</v>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
       <c r="O3" t="n">
         <v>7</v>
       </c>
@@ -865,7 +869,9 @@
       <c r="M4" t="n">
         <v>10810</v>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
       <c r="O4" t="n">
         <v>7</v>
       </c>
@@ -977,7 +983,9 @@
       <c r="M5" t="n">
         <v>21481</v>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
       <c r="O5" t="n">
         <v>7</v>
       </c>
@@ -1089,7 +1097,9 @@
       <c r="M6" t="n">
         <v>11653</v>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
       <c r="O6" t="n">
         <v>7</v>
       </c>
@@ -1201,7 +1211,9 @@
       <c r="M7" t="n">
         <v>32151</v>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
       <c r="O7" t="n">
         <v>7</v>
       </c>
@@ -1313,7 +1325,9 @@
       <c r="M8" t="n">
         <v>24570</v>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
       <c r="O8" t="n">
         <v>7</v>
       </c>
@@ -1423,7 +1437,9 @@
       <c r="M9" t="n">
         <v>47855</v>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
       <c r="O9" t="n">
         <v>7</v>
       </c>
@@ -1535,7 +1551,9 @@
       <c r="M10" t="n">
         <v>24830</v>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
       <c r="O10" t="n">
         <v>7</v>
       </c>
@@ -1647,7 +1665,9 @@
       <c r="M11" t="n">
         <v>105164</v>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
       <c r="O11" t="n">
         <v>5</v>
       </c>
@@ -1759,7 +1779,9 @@
       <c r="M12" t="n">
         <v>55000</v>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
       <c r="O12" t="n">
         <v>5</v>
       </c>
@@ -1869,7 +1891,9 @@
       <c r="M13" t="n">
         <v>50900</v>
       </c>
-      <c r="N13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
       <c r="O13" t="n">
         <v>7</v>
       </c>
@@ -1981,7 +2005,9 @@
       <c r="M14" t="n">
         <v>56900</v>
       </c>
-      <c r="N14" t="inlineStr"/>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
       <c r="O14" t="n">
         <v>7</v>
       </c>
@@ -2093,7 +2119,9 @@
       <c r="M15" t="n">
         <v>38400</v>
       </c>
-      <c r="N15" t="inlineStr"/>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
       <c r="O15" t="n">
         <v>10</v>
       </c>
@@ -2209,7 +2237,9 @@
       <c r="M16" t="n">
         <v>16900</v>
       </c>
-      <c r="N16" t="inlineStr"/>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
       <c r="O16" t="n">
         <v>7</v>
       </c>
@@ -2321,7 +2351,9 @@
       <c r="M17" t="n">
         <v>19500</v>
       </c>
-      <c r="N17" t="inlineStr"/>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
       <c r="O17" t="n">
         <v>7</v>
       </c>
@@ -2433,7 +2465,9 @@
       <c r="M18" t="n">
         <v>30145.79</v>
       </c>
-      <c r="N18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
       <c r="O18" t="n">
         <v>10</v>
       </c>
@@ -2549,7 +2583,9 @@
       <c r="M19" t="n">
         <v>18900</v>
       </c>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
       <c r="O19" t="n">
         <v>7</v>
       </c>
@@ -2665,7 +2701,9 @@
       <c r="M20" t="n">
         <v>13500</v>
       </c>
-      <c r="N20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
       <c r="O20" t="n">
         <v>10</v>
       </c>
@@ -2781,7 +2819,9 @@
       <c r="M21" t="n">
         <v>30450</v>
       </c>
-      <c r="N21" t="inlineStr"/>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
       <c r="O21" t="n">
         <v>10</v>
       </c>
@@ -2891,7 +2931,9 @@
       <c r="M22" t="n">
         <v>4300</v>
       </c>
-      <c r="N22" t="inlineStr"/>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
       <c r="O22" t="n">
         <v>7</v>
       </c>
@@ -3003,7 +3045,9 @@
       <c r="M23" t="n">
         <v>28288</v>
       </c>
-      <c r="N23" t="inlineStr"/>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
       <c r="O23" t="n">
         <v>7</v>
       </c>
@@ -3115,7 +3159,9 @@
       <c r="M24" t="n">
         <v>20199</v>
       </c>
-      <c r="N24" t="inlineStr"/>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
       <c r="O24" t="n">
         <v>7</v>
       </c>
@@ -3227,7 +3273,9 @@
       <c r="M25" t="n">
         <v>55106</v>
       </c>
-      <c r="N25" t="inlineStr"/>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
       <c r="O25" t="n">
         <v>10</v>
       </c>
@@ -3339,7 +3387,9 @@
       <c r="M26" t="n">
         <v>11700</v>
       </c>
-      <c r="N26" t="inlineStr"/>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
       <c r="O26" t="n">
         <v>10</v>
       </c>
@@ -3451,7 +3501,9 @@
       <c r="M27" t="n">
         <v>25920</v>
       </c>
-      <c r="N27" t="inlineStr"/>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
       <c r="O27" t="n">
         <v>10</v>
       </c>
@@ -3563,7 +3615,9 @@
       <c r="M28" t="n">
         <v>255360</v>
       </c>
-      <c r="N28" t="inlineStr"/>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
       <c r="O28" t="n">
         <v>10</v>
       </c>
@@ -3675,7 +3729,9 @@
       <c r="M29" t="n">
         <v>56300</v>
       </c>
-      <c r="N29" t="inlineStr"/>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
       <c r="O29" t="n">
         <v>7</v>
       </c>
@@ -3791,7 +3847,9 @@
       <c r="M30" t="n">
         <v>240000</v>
       </c>
-      <c r="N30" t="inlineStr"/>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
       <c r="O30" t="n">
         <v>10</v>
       </c>
@@ -3903,7 +3961,9 @@
       <c r="M31" t="n">
         <v>48000</v>
       </c>
-      <c r="N31" t="inlineStr"/>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
       <c r="O31" t="n">
         <v>10</v>
       </c>
@@ -4015,7 +4075,9 @@
       <c r="M32" t="n">
         <v>28800</v>
       </c>
-      <c r="N32" t="inlineStr"/>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
       <c r="O32" t="n">
         <v>10</v>
       </c>
@@ -4125,7 +4187,9 @@
       <c r="M33" t="n">
         <v>362600</v>
       </c>
-      <c r="N33" t="inlineStr"/>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
       <c r="O33" t="n">
         <v>7</v>
       </c>
@@ -4235,7 +4299,9 @@
       <c r="M34" t="n">
         <v>13375</v>
       </c>
-      <c r="N34" t="inlineStr"/>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
       <c r="O34" t="n">
         <v>10</v>
       </c>
@@ -4347,7 +4413,9 @@
       <c r="M35" t="n">
         <v>12300</v>
       </c>
-      <c r="N35" t="inlineStr"/>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
       <c r="O35" t="n">
         <v>7</v>
       </c>
@@ -4459,7 +4527,9 @@
       <c r="M36" t="n">
         <v>97300</v>
       </c>
-      <c r="N36" t="inlineStr"/>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
       <c r="O36" t="n">
         <v>10</v>
       </c>
@@ -4571,7 +4641,9 @@
       <c r="M37" t="n">
         <v>53770</v>
       </c>
-      <c r="N37" t="inlineStr"/>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
       <c r="O37" t="n">
         <v>7</v>
       </c>
@@ -4683,7 +4755,9 @@
       <c r="M38" t="n">
         <v>106500</v>
       </c>
-      <c r="N38" t="inlineStr"/>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
       <c r="O38" t="n">
         <v>7</v>
       </c>
@@ -4799,7 +4873,9 @@
       <c r="M39" t="n">
         <v>196000</v>
       </c>
-      <c r="N39" t="inlineStr"/>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
       <c r="O39" t="n">
         <v>7</v>
       </c>
@@ -4911,7 +4987,9 @@
       <c r="M40" t="n">
         <v>15000</v>
       </c>
-      <c r="N40" t="inlineStr"/>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
       <c r="O40" t="n">
         <v>10</v>
       </c>
@@ -5023,7 +5101,9 @@
       <c r="M41" t="n">
         <v>6375</v>
       </c>
-      <c r="N41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
       <c r="O41" t="n">
         <v>10</v>
       </c>
@@ -5135,7 +5215,9 @@
       <c r="M42" t="n">
         <v>16408</v>
       </c>
-      <c r="N42" t="inlineStr"/>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
       <c r="O42" t="n">
         <v>7</v>
       </c>
@@ -5247,7 +5329,9 @@
       <c r="M43" t="n">
         <v>12900</v>
       </c>
-      <c r="N43" t="inlineStr"/>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
       <c r="O43" t="n">
         <v>10</v>
       </c>
@@ -5363,7 +5447,9 @@
       <c r="M44" t="n">
         <v>11723.36</v>
       </c>
-      <c r="N44" t="inlineStr"/>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
       <c r="O44" t="n">
         <v>10</v>
       </c>
@@ -5475,7 +5561,9 @@
       <c r="M45" t="n">
         <v>2930.84</v>
       </c>
-      <c r="N45" t="inlineStr"/>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
       <c r="O45" t="n">
         <v>10</v>
       </c>
@@ -5587,7 +5675,9 @@
       <c r="M46" t="n">
         <v>10400</v>
       </c>
-      <c r="N46" t="inlineStr"/>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
       <c r="O46" t="n">
         <v>7</v>
       </c>
@@ -5697,7 +5787,9 @@
       <c r="M47" t="n">
         <v>80250</v>
       </c>
-      <c r="N47" t="inlineStr"/>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
       <c r="O47" t="n">
         <v>7</v>
       </c>
@@ -5809,7 +5901,9 @@
       <c r="M48" t="n">
         <v>48215</v>
       </c>
-      <c r="N48" t="inlineStr"/>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
       <c r="O48" t="n">
         <v>10</v>
       </c>
@@ -5925,7 +6019,9 @@
       <c r="M49" t="n">
         <v>54124</v>
       </c>
-      <c r="N49" t="inlineStr"/>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
       <c r="O49" t="n">
         <v>7</v>
       </c>
@@ -6041,7 +6137,9 @@
       <c r="M50" t="n">
         <v>97240</v>
       </c>
-      <c r="N50" t="inlineStr"/>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
       <c r="O50" t="n">
         <v>10</v>
       </c>
@@ -6157,7 +6255,9 @@
       <c r="M51" t="n">
         <v>167000</v>
       </c>
-      <c r="N51" t="inlineStr"/>
+      <c r="N51" t="n">
+        <v>0</v>
+      </c>
       <c r="O51" t="n">
         <v>7</v>
       </c>
@@ -6273,7 +6373,9 @@
       <c r="M52" t="n">
         <v>385050</v>
       </c>
-      <c r="N52" t="inlineStr"/>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
       <c r="O52" t="n">
         <v>7</v>
       </c>
@@ -6389,7 +6491,9 @@
       <c r="M53" t="n">
         <v>119900</v>
       </c>
-      <c r="N53" t="inlineStr"/>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
       <c r="O53" t="n">
         <v>10</v>
       </c>
@@ -6505,7 +6609,9 @@
       <c r="M54" t="n">
         <v>57021</v>
       </c>
-      <c r="N54" t="inlineStr"/>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
       <c r="O54" t="n">
         <v>10</v>
       </c>
@@ -6621,7 +6727,9 @@
       <c r="M55" t="n">
         <v>13789.8</v>
       </c>
-      <c r="N55" t="inlineStr"/>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
       <c r="O55" t="n">
         <v>10</v>
       </c>
@@ -6737,7 +6845,9 @@
       <c r="M56" t="n">
         <v>6550</v>
       </c>
-      <c r="N56" t="inlineStr"/>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
       <c r="O56" t="n">
         <v>10</v>
       </c>
@@ -6853,7 +6963,9 @@
       <c r="M57" t="n">
         <v>27379</v>
       </c>
-      <c r="N57" t="inlineStr"/>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
       <c r="O57" t="n">
         <v>10</v>
       </c>
@@ -6969,7 +7081,9 @@
       <c r="M58" t="n">
         <v>57400</v>
       </c>
-      <c r="N58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
       <c r="O58" t="n">
         <v>10</v>
       </c>
@@ -7085,7 +7199,9 @@
       <c r="M59" t="n">
         <v>36220</v>
       </c>
-      <c r="N59" t="inlineStr"/>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
       <c r="O59" t="n">
         <v>10</v>
       </c>
@@ -7201,7 +7317,9 @@
       <c r="M60" t="n">
         <v>101042</v>
       </c>
-      <c r="N60" t="inlineStr"/>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
       <c r="O60" t="n">
         <v>10</v>
       </c>
@@ -7317,7 +7435,9 @@
       <c r="M61" t="n">
         <v>83200</v>
       </c>
-      <c r="N61" t="inlineStr"/>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
       <c r="O61" t="n">
         <v>5</v>
       </c>
@@ -7429,7 +7549,9 @@
       <c r="M62" t="n">
         <v>146100</v>
       </c>
-      <c r="N62" t="inlineStr"/>
+      <c r="N62" t="n">
+        <v>0</v>
+      </c>
       <c r="O62" t="n">
         <v>5</v>
       </c>
@@ -7541,7 +7663,9 @@
       <c r="M63" t="n">
         <v>18368</v>
       </c>
-      <c r="N63" t="inlineStr"/>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
       <c r="O63" t="n">
         <v>7</v>
       </c>
@@ -7653,7 +7777,9 @@
       <c r="M64" t="n">
         <v>17072.14</v>
       </c>
-      <c r="N64" t="inlineStr"/>
+      <c r="N64" t="n">
+        <v>0</v>
+      </c>
       <c r="O64" t="n">
         <v>10</v>
       </c>
@@ -7765,7 +7891,9 @@
       <c r="M65" t="n">
         <v>90000</v>
       </c>
-      <c r="N65" t="inlineStr"/>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
       <c r="O65" t="n">
         <v>10</v>
       </c>
@@ -7881,7 +8009,9 @@
       <c r="M66" t="n">
         <v>197600</v>
       </c>
-      <c r="N66" t="inlineStr"/>
+      <c r="N66" t="n">
+        <v>0</v>
+      </c>
       <c r="O66" t="n">
         <v>5</v>
       </c>
@@ -7993,7 +8123,9 @@
       <c r="M67" t="n">
         <v>57700</v>
       </c>
-      <c r="N67" t="inlineStr"/>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
       <c r="O67" t="n">
         <v>5</v>
       </c>
@@ -8105,7 +8237,9 @@
       <c r="M68" t="n">
         <v>55000</v>
       </c>
-      <c r="N68" t="inlineStr"/>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
       <c r="O68" t="n">
         <v>10</v>
       </c>
@@ -8217,7 +8351,9 @@
       <c r="M69" t="n">
         <v>25000</v>
       </c>
-      <c r="N69" t="inlineStr"/>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
       <c r="O69" t="n">
         <v>10</v>
       </c>
@@ -8329,7 +8465,9 @@
       <c r="M70" t="n">
         <v>46980</v>
       </c>
-      <c r="N70" t="inlineStr"/>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
       <c r="O70" t="n">
         <v>10</v>
       </c>
@@ -8445,7 +8583,9 @@
       <c r="M71" t="n">
         <v>7330</v>
       </c>
-      <c r="N71" t="inlineStr"/>
+      <c r="N71" t="n">
+        <v>0</v>
+      </c>
       <c r="O71" t="n">
         <v>10</v>
       </c>
@@ -8557,7 +8697,9 @@
       <c r="M72" t="n">
         <v>46000</v>
       </c>
-      <c r="N72" t="inlineStr"/>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
       <c r="O72" t="n">
         <v>5</v>
       </c>
@@ -8669,7 +8811,9 @@
       <c r="M73" t="n">
         <v>9500</v>
       </c>
-      <c r="N73" t="inlineStr"/>
+      <c r="N73" t="n">
+        <v>0</v>
+      </c>
       <c r="O73" t="n">
         <v>10</v>
       </c>
@@ -8781,7 +8925,9 @@
       <c r="M74" t="n">
         <v>16800</v>
       </c>
-      <c r="N74" t="inlineStr"/>
+      <c r="N74" t="n">
+        <v>0</v>
+      </c>
       <c r="O74" t="n">
         <v>10</v>
       </c>
@@ -8893,7 +9039,9 @@
       <c r="M75" t="n">
         <v>12750</v>
       </c>
-      <c r="N75" t="inlineStr"/>
+      <c r="N75" t="n">
+        <v>0</v>
+      </c>
       <c r="O75" t="n">
         <v>10</v>
       </c>
@@ -9005,7 +9153,9 @@
       <c r="M76" t="n">
         <v>31500</v>
       </c>
-      <c r="N76" t="inlineStr"/>
+      <c r="N76" t="n">
+        <v>0</v>
+      </c>
       <c r="O76" t="n">
         <v>10</v>
       </c>
@@ -9115,7 +9265,9 @@
       <c r="M77" t="n">
         <v>20662</v>
       </c>
-      <c r="N77" t="inlineStr"/>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
       <c r="O77" t="n">
         <v>7</v>
       </c>
@@ -9227,7 +9379,9 @@
       <c r="M78" t="n">
         <v>16963</v>
       </c>
-      <c r="N78" t="inlineStr"/>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
       <c r="O78" t="n">
         <v>10</v>
       </c>
@@ -9339,7 +9493,9 @@
       <c r="M79" t="n">
         <v>12000</v>
       </c>
-      <c r="N79" t="inlineStr"/>
+      <c r="N79" t="n">
+        <v>0</v>
+      </c>
       <c r="O79" t="n">
         <v>10</v>
       </c>
@@ -9451,7 +9607,9 @@
       <c r="M80" t="n">
         <v>5000</v>
       </c>
-      <c r="N80" t="inlineStr"/>
+      <c r="N80" t="n">
+        <v>0</v>
+      </c>
       <c r="O80" t="n">
         <v>10</v>
       </c>
@@ -9563,7 +9721,9 @@
       <c r="M81" t="n">
         <v>63665</v>
       </c>
-      <c r="N81" t="inlineStr"/>
+      <c r="N81" t="n">
+        <v>0</v>
+      </c>
       <c r="O81" t="n">
         <v>5</v>
       </c>
@@ -9675,7 +9835,9 @@
       <c r="M82" t="n">
         <v>3745</v>
       </c>
-      <c r="N82" t="inlineStr"/>
+      <c r="N82" t="n">
+        <v>0</v>
+      </c>
       <c r="O82" t="n">
         <v>5</v>
       </c>
@@ -9787,7 +9949,9 @@
       <c r="M83" t="n">
         <v>18725</v>
       </c>
-      <c r="N83" t="inlineStr"/>
+      <c r="N83" t="n">
+        <v>0</v>
+      </c>
       <c r="O83" t="n">
         <v>5</v>
       </c>
@@ -9899,7 +10063,9 @@
       <c r="M84" t="n">
         <v>28890</v>
       </c>
-      <c r="N84" t="inlineStr"/>
+      <c r="N84" t="n">
+        <v>0</v>
+      </c>
       <c r="O84" t="n">
         <v>5</v>
       </c>
@@ -10011,7 +10177,9 @@
       <c r="M85" t="n">
         <v>39380</v>
       </c>
-      <c r="N85" t="inlineStr"/>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
       <c r="O85" t="n">
         <v>7</v>
       </c>
@@ -10123,7 +10291,9 @@
       <c r="M86" t="n">
         <v>15194</v>
       </c>
-      <c r="N86" t="inlineStr"/>
+      <c r="N86" t="n">
+        <v>0</v>
+      </c>
       <c r="O86" t="n">
         <v>5</v>
       </c>
@@ -10235,7 +10405,9 @@
       <c r="M87" t="n">
         <v>5350</v>
       </c>
-      <c r="N87" t="inlineStr"/>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
       <c r="O87" t="n">
         <v>5</v>
       </c>
@@ -10347,7 +10519,9 @@
       <c r="M88" t="n">
         <v>62500</v>
       </c>
-      <c r="N88" t="inlineStr"/>
+      <c r="N88" t="n">
+        <v>0</v>
+      </c>
       <c r="O88" t="n">
         <v>7</v>
       </c>
@@ -10459,7 +10633,9 @@
       <c r="M89" t="n">
         <v>12305</v>
       </c>
-      <c r="N89" t="inlineStr"/>
+      <c r="N89" t="n">
+        <v>0</v>
+      </c>
       <c r="O89" t="n">
         <v>5</v>
       </c>
@@ -10571,7 +10747,9 @@
       <c r="M90" t="n">
         <v>172056</v>
       </c>
-      <c r="N90" t="inlineStr"/>
+      <c r="N90" t="n">
+        <v>0</v>
+      </c>
       <c r="O90" t="n">
         <v>5</v>
       </c>
@@ -10683,7 +10861,9 @@
       <c r="M91" t="n">
         <v>5564</v>
       </c>
-      <c r="N91" t="inlineStr"/>
+      <c r="N91" t="n">
+        <v>0</v>
+      </c>
       <c r="O91" t="n">
         <v>5</v>
       </c>
@@ -10795,7 +10975,9 @@
       <c r="M92" t="n">
         <v>311168</v>
       </c>
-      <c r="N92" t="inlineStr"/>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
       <c r="O92" t="n">
         <v>10</v>
       </c>
@@ -10911,7 +11093,9 @@
       <c r="M93" t="n">
         <v>60480</v>
       </c>
-      <c r="N93" t="inlineStr"/>
+      <c r="N93" t="n">
+        <v>0</v>
+      </c>
       <c r="O93" t="n">
         <v>10</v>
       </c>
@@ -11027,7 +11211,9 @@
       <c r="M94" t="n">
         <v>14000</v>
       </c>
-      <c r="N94" t="inlineStr"/>
+      <c r="N94" t="n">
+        <v>0</v>
+      </c>
       <c r="O94" t="n">
         <v>10</v>
       </c>
@@ -11143,7 +11329,9 @@
       <c r="M95" t="n">
         <v>337568</v>
       </c>
-      <c r="N95" t="inlineStr"/>
+      <c r="N95" t="n">
+        <v>0</v>
+      </c>
       <c r="O95" t="n">
         <v>7</v>
       </c>
@@ -11257,7 +11445,9 @@
       <c r="M96" t="n">
         <v>35000</v>
       </c>
-      <c r="N96" t="inlineStr"/>
+      <c r="N96" t="n">
+        <v>0</v>
+      </c>
       <c r="O96" t="n">
         <v>10</v>
       </c>
@@ -11369,7 +11559,9 @@
       <c r="M97" t="n">
         <v>36700</v>
       </c>
-      <c r="N97" t="inlineStr"/>
+      <c r="N97" t="n">
+        <v>0</v>
+      </c>
       <c r="O97" t="n">
         <v>7</v>
       </c>
@@ -11479,7 +11671,9 @@
       <c r="M98" t="n">
         <v>214136</v>
       </c>
-      <c r="N98" t="inlineStr"/>
+      <c r="N98" t="n">
+        <v>0</v>
+      </c>
       <c r="O98" t="n">
         <v>7</v>
       </c>
@@ -11591,7 +11785,9 @@
       <c r="M99" t="n">
         <v>9276465</v>
       </c>
-      <c r="N99" t="inlineStr"/>
+      <c r="N99" t="n">
+        <v>0</v>
+      </c>
       <c r="O99" t="n">
         <v>10</v>
       </c>
@@ -11703,7 +11899,9 @@
       <c r="M100" t="n">
         <v>9046900</v>
       </c>
-      <c r="N100" t="inlineStr"/>
+      <c r="N100" t="n">
+        <v>0</v>
+      </c>
       <c r="O100" t="n">
         <v>10</v>
       </c>
@@ -11815,7 +12013,9 @@
       <c r="M101" t="n">
         <v>42801</v>
       </c>
-      <c r="N101" t="inlineStr"/>
+      <c r="N101" t="n">
+        <v>0</v>
+      </c>
       <c r="O101" t="n">
         <v>7</v>
       </c>
@@ -11927,7 +12127,9 @@
       <c r="M102" t="n">
         <v>20100</v>
       </c>
-      <c r="N102" t="inlineStr"/>
+      <c r="N102" t="n">
+        <v>0</v>
+      </c>
       <c r="O102" t="n">
         <v>7</v>
       </c>
@@ -12039,7 +12241,9 @@
       <c r="M103" t="n">
         <v>4320</v>
       </c>
-      <c r="N103" t="inlineStr"/>
+      <c r="N103" t="n">
+        <v>0</v>
+      </c>
       <c r="O103" t="n">
         <v>7</v>
       </c>
@@ -12151,7 +12355,9 @@
       <c r="M104" t="n">
         <v>186384</v>
       </c>
-      <c r="N104" t="inlineStr"/>
+      <c r="N104" t="n">
+        <v>0</v>
+      </c>
       <c r="O104" t="n">
         <v>7</v>
       </c>
@@ -12265,7 +12471,9 @@
       <c r="M105" t="n">
         <v>9900</v>
       </c>
-      <c r="N105" t="inlineStr"/>
+      <c r="N105" t="n">
+        <v>0</v>
+      </c>
       <c r="O105" t="n">
         <v>7</v>
       </c>
@@ -12377,7 +12585,9 @@
       <c r="M106" t="n">
         <v>57800</v>
       </c>
-      <c r="N106" t="inlineStr"/>
+      <c r="N106" t="n">
+        <v>0</v>
+      </c>
       <c r="O106" t="n">
         <v>7</v>
       </c>
@@ -12489,7 +12699,9 @@
       <c r="M107" t="n">
         <v>374075</v>
       </c>
-      <c r="N107" t="inlineStr"/>
+      <c r="N107" t="n">
+        <v>0</v>
+      </c>
       <c r="O107" t="n">
         <v>7</v>
       </c>
@@ -12605,7 +12817,9 @@
       <c r="M108" t="n">
         <v>182937</v>
       </c>
-      <c r="N108" t="inlineStr"/>
+      <c r="N108" t="n">
+        <v>0</v>
+      </c>
       <c r="O108" t="n">
         <v>7</v>
       </c>
@@ -12717,7 +12931,9 @@
       <c r="M109" t="n">
         <v>9146</v>
       </c>
-      <c r="N109" t="inlineStr"/>
+      <c r="N109" t="n">
+        <v>0</v>
+      </c>
       <c r="O109" t="n">
         <v>7</v>
       </c>
@@ -12829,7 +13045,9 @@
       <c r="M110" t="n">
         <v>72760</v>
       </c>
-      <c r="N110" t="inlineStr"/>
+      <c r="N110" t="n">
+        <v>0</v>
+      </c>
       <c r="O110" t="n">
         <v>7</v>
       </c>
@@ -12941,7 +13159,9 @@
       <c r="M111" t="n">
         <v>68448</v>
       </c>
-      <c r="N111" t="inlineStr"/>
+      <c r="N111" t="n">
+        <v>0</v>
+      </c>
       <c r="O111" t="n">
         <v>10</v>
       </c>
@@ -13057,7 +13277,9 @@
       <c r="M112" t="n">
         <v>35910</v>
       </c>
-      <c r="N112" t="inlineStr"/>
+      <c r="N112" t="n">
+        <v>0</v>
+      </c>
       <c r="O112" t="n">
         <v>10</v>
       </c>
@@ -13173,7 +13395,9 @@
       <c r="M113" t="n">
         <v>22500</v>
       </c>
-      <c r="N113" t="inlineStr"/>
+      <c r="N113" t="n">
+        <v>0</v>
+      </c>
       <c r="O113" t="n">
         <v>10</v>
       </c>
@@ -13289,7 +13513,9 @@
       <c r="M114" t="n">
         <v>98000</v>
       </c>
-      <c r="N114" t="inlineStr"/>
+      <c r="N114" t="n">
+        <v>0</v>
+      </c>
       <c r="O114" t="n">
         <v>10</v>
       </c>
@@ -13405,7 +13631,9 @@
       <c r="M115" t="n">
         <v>294000</v>
       </c>
-      <c r="N115" t="inlineStr"/>
+      <c r="N115" t="n">
+        <v>0</v>
+      </c>
       <c r="O115" t="n">
         <v>10</v>
       </c>
@@ -13517,7 +13745,9 @@
       <c r="M116" t="n">
         <v>14000</v>
       </c>
-      <c r="N116" t="inlineStr"/>
+      <c r="N116" t="n">
+        <v>0</v>
+      </c>
       <c r="O116" t="n">
         <v>10</v>
       </c>
@@ -13629,7 +13859,9 @@
       <c r="M117" t="n">
         <v>51939</v>
       </c>
-      <c r="N117" t="inlineStr"/>
+      <c r="N117" t="n">
+        <v>0</v>
+      </c>
       <c r="O117" t="n">
         <v>7</v>
       </c>
@@ -13741,7 +13973,9 @@
       <c r="M118" t="n">
         <v>48870</v>
       </c>
-      <c r="N118" t="inlineStr"/>
+      <c r="N118" t="n">
+        <v>0</v>
+      </c>
       <c r="O118" t="n">
         <v>10</v>
       </c>
@@ -13857,7 +14091,9 @@
       <c r="M119" t="n">
         <v>22520</v>
       </c>
-      <c r="N119" t="inlineStr"/>
+      <c r="N119" t="n">
+        <v>0</v>
+      </c>
       <c r="O119" t="n">
         <v>10</v>
       </c>
@@ -13969,7 +14205,9 @@
       <c r="M120" t="n">
         <v>24900</v>
       </c>
-      <c r="N120" t="inlineStr"/>
+      <c r="N120" t="n">
+        <v>0</v>
+      </c>
       <c r="O120" t="n">
         <v>7</v>
       </c>
@@ -14081,7 +14319,9 @@
       <c r="M121" t="n">
         <v>48485</v>
       </c>
-      <c r="N121" t="inlineStr"/>
+      <c r="N121" t="n">
+        <v>0</v>
+      </c>
       <c r="O121" t="n">
         <v>7</v>
       </c>
@@ -14193,7 +14433,9 @@
       <c r="M122" t="n">
         <v>33172</v>
       </c>
-      <c r="N122" t="inlineStr"/>
+      <c r="N122" t="n">
+        <v>0</v>
+      </c>
       <c r="O122" t="n">
         <v>10</v>
       </c>
@@ -14305,7 +14547,9 @@
       <c r="M123" t="n">
         <v>87706.17</v>
       </c>
-      <c r="N123" t="inlineStr"/>
+      <c r="N123" t="n">
+        <v>0</v>
+      </c>
       <c r="O123" t="n">
         <v>5</v>
       </c>
@@ -14417,7 +14661,9 @@
       <c r="M124" t="n">
         <v>106113.64</v>
       </c>
-      <c r="N124" t="inlineStr"/>
+      <c r="N124" t="n">
+        <v>0</v>
+      </c>
       <c r="O124" t="n">
         <v>5</v>
       </c>
@@ -14529,7 +14775,9 @@
       <c r="M125" t="n">
         <v>44394.48</v>
       </c>
-      <c r="N125" t="inlineStr"/>
+      <c r="N125" t="n">
+        <v>0</v>
+      </c>
       <c r="O125" t="n">
         <v>5</v>
       </c>
@@ -14641,7 +14889,9 @@
       <c r="M126" t="n">
         <v>7254.71</v>
       </c>
-      <c r="N126" t="inlineStr"/>
+      <c r="N126" t="n">
+        <v>0</v>
+      </c>
       <c r="O126" t="n">
         <v>5</v>
       </c>
@@ -14753,7 +15003,9 @@
       <c r="M127" t="n">
         <v>29000</v>
       </c>
-      <c r="N127" t="inlineStr"/>
+      <c r="N127" t="n">
+        <v>0</v>
+      </c>
       <c r="O127" t="n">
         <v>10</v>
       </c>
@@ -14865,7 +15117,9 @@
       <c r="M128" t="n">
         <v>117000</v>
       </c>
-      <c r="N128" t="inlineStr"/>
+      <c r="N128" t="n">
+        <v>0</v>
+      </c>
       <c r="O128" t="n">
         <v>10</v>
       </c>
@@ -14977,7 +15231,9 @@
       <c r="M129" t="n">
         <v>17500</v>
       </c>
-      <c r="N129" t="inlineStr"/>
+      <c r="N129" t="n">
+        <v>0</v>
+      </c>
       <c r="O129" t="n">
         <v>10</v>
       </c>
@@ -15089,7 +15345,9 @@
       <c r="M130" t="n">
         <v>20442</v>
       </c>
-      <c r="N130" t="inlineStr"/>
+      <c r="N130" t="n">
+        <v>0</v>
+      </c>
       <c r="O130" t="n">
         <v>5</v>
       </c>
@@ -15201,7 +15459,9 @@
       <c r="M131" t="n">
         <v>56354</v>
       </c>
-      <c r="N131" t="inlineStr"/>
+      <c r="N131" t="n">
+        <v>0</v>
+      </c>
       <c r="O131" t="n">
         <v>5</v>
       </c>
@@ -15313,7 +15573,9 @@
       <c r="M132" t="n">
         <v>41989</v>
       </c>
-      <c r="N132" t="inlineStr"/>
+      <c r="N132" t="n">
+        <v>0</v>
+      </c>
       <c r="O132" t="n">
         <v>5</v>
       </c>
@@ -15425,7 +15687,9 @@
       <c r="M133" t="n">
         <v>1989</v>
       </c>
-      <c r="N133" t="inlineStr"/>
+      <c r="N133" t="n">
+        <v>0</v>
+      </c>
       <c r="O133" t="n">
         <v>5</v>
       </c>
@@ -15537,7 +15801,9 @@
       <c r="M134" t="n">
         <v>9075</v>
       </c>
-      <c r="N134" t="inlineStr"/>
+      <c r="N134" t="n">
+        <v>0</v>
+      </c>
       <c r="O134" t="n">
         <v>7</v>
       </c>
@@ -15649,7 +15915,9 @@
       <c r="M135" t="n">
         <v>81400</v>
       </c>
-      <c r="N135" t="inlineStr"/>
+      <c r="N135" t="n">
+        <v>0</v>
+      </c>
       <c r="O135" t="n">
         <v>5</v>
       </c>
@@ -15761,7 +16029,9 @@
       <c r="M136" t="n">
         <v>23980</v>
       </c>
-      <c r="N136" t="inlineStr"/>
+      <c r="N136" t="n">
+        <v>0</v>
+      </c>
       <c r="O136" t="n">
         <v>5</v>
       </c>
@@ -15873,7 +16143,9 @@
       <c r="M137" t="n">
         <v>9900</v>
       </c>
-      <c r="N137" t="inlineStr"/>
+      <c r="N137" t="n">
+        <v>0</v>
+      </c>
       <c r="O137" t="n">
         <v>5</v>
       </c>
@@ -15985,7 +16257,9 @@
       <c r="M138" t="n">
         <v>133335</v>
       </c>
-      <c r="N138" t="inlineStr"/>
+      <c r="N138" t="n">
+        <v>0</v>
+      </c>
       <c r="O138" t="n">
         <v>5</v>
       </c>
@@ -16097,7 +16371,9 @@
       <c r="M139" t="n">
         <v>17814</v>
       </c>
-      <c r="N139" t="inlineStr"/>
+      <c r="N139" t="n">
+        <v>0</v>
+      </c>
       <c r="O139" t="n">
         <v>10</v>
       </c>
@@ -16209,7 +16485,9 @@
       <c r="M140" t="n">
         <v>59116</v>
       </c>
-      <c r="N140" t="inlineStr"/>
+      <c r="N140" t="n">
+        <v>0</v>
+      </c>
       <c r="O140" t="n">
         <v>5</v>
       </c>
@@ -16321,7 +16599,9 @@
       <c r="M141" t="n">
         <v>4500</v>
       </c>
-      <c r="N141" t="inlineStr"/>
+      <c r="N141" t="n">
+        <v>0</v>
+      </c>
       <c r="O141" t="n">
         <v>10</v>
       </c>
@@ -16433,7 +16713,9 @@
       <c r="M142" t="n">
         <v>279005</v>
       </c>
-      <c r="N142" t="inlineStr"/>
+      <c r="N142" t="n">
+        <v>0</v>
+      </c>
       <c r="O142" t="n">
         <v>5</v>
       </c>
@@ -16545,7 +16827,9 @@
       <c r="M143" t="n">
         <v>130387</v>
       </c>
-      <c r="N143" t="inlineStr"/>
+      <c r="N143" t="n">
+        <v>0</v>
+      </c>
       <c r="O143" t="n">
         <v>5</v>
       </c>
@@ -16657,7 +16941,9 @@
       <c r="M144" t="n">
         <v>3296500</v>
       </c>
-      <c r="N144" t="inlineStr"/>
+      <c r="N144" t="n">
+        <v>0</v>
+      </c>
       <c r="O144" t="n">
         <v>10</v>
       </c>
@@ -16767,7 +17053,9 @@
       <c r="M145" t="n">
         <v>30331</v>
       </c>
-      <c r="N145" t="inlineStr"/>
+      <c r="N145" t="n">
+        <v>0</v>
+      </c>
       <c r="O145" t="n">
         <v>10</v>
       </c>
@@ -16879,7 +17167,9 @@
       <c r="M146" t="n">
         <v>161000</v>
       </c>
-      <c r="N146" t="inlineStr"/>
+      <c r="N146" t="n">
+        <v>0</v>
+      </c>
       <c r="O146" t="n">
         <v>7</v>
       </c>
@@ -16991,7 +17281,9 @@
       <c r="M147" t="n">
         <v>82123.02</v>
       </c>
-      <c r="N147" t="inlineStr"/>
+      <c r="N147" t="n">
+        <v>0</v>
+      </c>
       <c r="O147" t="n">
         <v>5</v>
       </c>
@@ -17103,7 +17395,9 @@
       <c r="M148" t="n">
         <v>32402.28</v>
       </c>
-      <c r="N148" t="inlineStr"/>
+      <c r="N148" t="n">
+        <v>0</v>
+      </c>
       <c r="O148" t="n">
         <v>5</v>
       </c>
@@ -17213,7 +17507,9 @@
       <c r="M149" t="n">
         <v>21450</v>
       </c>
-      <c r="N149" t="inlineStr"/>
+      <c r="N149" t="n">
+        <v>0</v>
+      </c>
       <c r="O149" t="n">
         <v>10</v>
       </c>
@@ -17325,7 +17621,9 @@
       <c r="M150" t="n">
         <v>19485</v>
       </c>
-      <c r="N150" t="inlineStr"/>
+      <c r="N150" t="n">
+        <v>0</v>
+      </c>
       <c r="O150" t="n">
         <v>10</v>
       </c>
@@ -17437,7 +17735,9 @@
       <c r="M151" t="n">
         <v>4500</v>
       </c>
-      <c r="N151" t="inlineStr"/>
+      <c r="N151" t="n">
+        <v>0</v>
+      </c>
       <c r="O151" t="n">
         <v>7</v>
       </c>
@@ -17551,7 +17851,9 @@
       <c r="M152" t="n">
         <v>10000</v>
       </c>
-      <c r="N152" t="inlineStr"/>
+      <c r="N152" t="n">
+        <v>0</v>
+      </c>
       <c r="O152" t="n">
         <v>20</v>
       </c>
@@ -17665,7 +17967,9 @@
       <c r="M153" t="n">
         <v>10000</v>
       </c>
-      <c r="N153" t="inlineStr"/>
+      <c r="N153" t="n">
+        <v>0</v>
+      </c>
       <c r="O153" t="n">
         <v>20</v>
       </c>
@@ -17779,7 +18083,9 @@
       <c r="M154" t="n">
         <v>79259.95</v>
       </c>
-      <c r="N154" t="inlineStr"/>
+      <c r="N154" t="n">
+        <v>0</v>
+      </c>
       <c r="O154" t="n">
         <v>20</v>
       </c>
@@ -17893,7 +18199,9 @@
       <c r="M155" t="n">
         <v>26387.5</v>
       </c>
-      <c r="N155" t="inlineStr"/>
+      <c r="N155" t="n">
+        <v>0</v>
+      </c>
       <c r="O155" t="n">
         <v>20</v>
       </c>
@@ -18007,7 +18315,9 @@
       <c r="M156" t="n">
         <v>3979.25</v>
       </c>
-      <c r="N156" t="inlineStr"/>
+      <c r="N156" t="n">
+        <v>0</v>
+      </c>
       <c r="O156" t="n">
         <v>20</v>
       </c>
@@ -18121,7 +18431,9 @@
       <c r="M157" t="n">
         <v>250000</v>
       </c>
-      <c r="N157" t="inlineStr"/>
+      <c r="N157" t="n">
+        <v>0</v>
+      </c>
       <c r="O157" t="n">
         <v>20</v>
       </c>
@@ -18235,7 +18547,9 @@
       <c r="M158" t="n">
         <v>38500</v>
       </c>
-      <c r="N158" t="inlineStr"/>
+      <c r="N158" t="n">
+        <v>0</v>
+      </c>
       <c r="O158" t="n">
         <v>20</v>
       </c>
@@ -18349,7 +18663,9 @@
       <c r="M159" t="n">
         <v>1396.5</v>
       </c>
-      <c r="N159" t="inlineStr"/>
+      <c r="N159" t="n">
+        <v>0</v>
+      </c>
       <c r="O159" t="n">
         <v>20</v>
       </c>
@@ -18463,7 +18779,9 @@
       <c r="M160" t="n">
         <v>124300</v>
       </c>
-      <c r="N160" t="inlineStr"/>
+      <c r="N160" t="n">
+        <v>0</v>
+      </c>
       <c r="O160" t="n">
         <v>20</v>
       </c>
@@ -18577,7 +18895,9 @@
       <c r="M161" t="n">
         <v>5475</v>
       </c>
-      <c r="N161" t="inlineStr"/>
+      <c r="N161" t="n">
+        <v>0</v>
+      </c>
       <c r="O161" t="n">
         <v>20</v>
       </c>
@@ -18691,7 +19011,9 @@
       <c r="M162" t="n">
         <v>328860</v>
       </c>
-      <c r="N162" t="inlineStr"/>
+      <c r="N162" t="n">
+        <v>0</v>
+      </c>
       <c r="O162" t="n">
         <v>15</v>
       </c>
@@ -18805,7 +19127,9 @@
       <c r="M163" t="n">
         <v>38150</v>
       </c>
-      <c r="N163" t="inlineStr"/>
+      <c r="N163" t="n">
+        <v>0</v>
+      </c>
       <c r="O163" t="n">
         <v>15</v>
       </c>
@@ -18919,7 +19243,9 @@
       <c r="M164" t="n">
         <v>35000</v>
       </c>
-      <c r="N164" t="inlineStr"/>
+      <c r="N164" t="n">
+        <v>0</v>
+      </c>
       <c r="O164" t="n">
         <v>15</v>
       </c>
@@ -19033,7 +19359,9 @@
       <c r="M165" t="n">
         <v>38150</v>
       </c>
-      <c r="N165" t="inlineStr"/>
+      <c r="N165" t="n">
+        <v>0</v>
+      </c>
       <c r="O165" t="n">
         <v>15</v>
       </c>
@@ -19147,7 +19475,9 @@
       <c r="M166" t="n">
         <v>1190</v>
       </c>
-      <c r="N166" t="inlineStr"/>
+      <c r="N166" t="n">
+        <v>0</v>
+      </c>
       <c r="O166" t="n">
         <v>15</v>
       </c>
@@ -19261,7 +19591,9 @@
       <c r="M167" t="n">
         <v>7500</v>
       </c>
-      <c r="N167" t="inlineStr"/>
+      <c r="N167" t="n">
+        <v>0</v>
+      </c>
       <c r="O167" t="n">
         <v>15</v>
       </c>
@@ -19375,7 +19707,9 @@
       <c r="M168" t="n">
         <v>31005</v>
       </c>
-      <c r="N168" t="inlineStr"/>
+      <c r="N168" t="n">
+        <v>0</v>
+      </c>
       <c r="O168" t="n">
         <v>15</v>
       </c>
@@ -19490,7 +19824,9 @@
       <c r="M169" t="n">
         <v>7000</v>
       </c>
-      <c r="N169" t="inlineStr"/>
+      <c r="N169" t="n">
+        <v>0</v>
+      </c>
       <c r="O169" t="n">
         <v>15</v>
       </c>
@@ -19604,7 +19940,9 @@
       <c r="M170" t="n">
         <v>55000</v>
       </c>
-      <c r="N170" t="inlineStr"/>
+      <c r="N170" t="n">
+        <v>0</v>
+      </c>
       <c r="O170" t="n">
         <v>15</v>
       </c>
@@ -19718,7 +20056,9 @@
       <c r="M171" t="n">
         <v>134000</v>
       </c>
-      <c r="N171" t="inlineStr"/>
+      <c r="N171" t="n">
+        <v>0</v>
+      </c>
       <c r="O171" t="n">
         <v>15</v>
       </c>
@@ -19832,7 +20172,9 @@
       <c r="M172" t="n">
         <v>42500</v>
       </c>
-      <c r="N172" t="inlineStr"/>
+      <c r="N172" t="n">
+        <v>0</v>
+      </c>
       <c r="O172" t="n">
         <v>15</v>
       </c>
@@ -19946,7 +20288,9 @@
       <c r="M173" t="n">
         <v>147000</v>
       </c>
-      <c r="N173" t="inlineStr"/>
+      <c r="N173" t="n">
+        <v>0</v>
+      </c>
       <c r="O173" t="n">
         <v>20</v>
       </c>
@@ -20060,7 +20404,9 @@
       <c r="M174" t="n">
         <v>210600</v>
       </c>
-      <c r="N174" t="inlineStr"/>
+      <c r="N174" t="n">
+        <v>0</v>
+      </c>
       <c r="O174" t="n">
         <v>20</v>
       </c>
@@ -20174,7 +20520,9 @@
       <c r="M175" t="n">
         <v>7180</v>
       </c>
-      <c r="N175" t="inlineStr"/>
+      <c r="N175" t="n">
+        <v>0</v>
+      </c>
       <c r="O175" t="n">
         <v>20</v>
       </c>
@@ -20288,7 +20636,9 @@
       <c r="M176" t="n">
         <v>5850</v>
       </c>
-      <c r="N176" t="inlineStr"/>
+      <c r="N176" t="n">
+        <v>0</v>
+      </c>
       <c r="O176" t="n">
         <v>20</v>
       </c>
@@ -20402,7 +20752,9 @@
       <c r="M177" t="n">
         <v>9000</v>
       </c>
-      <c r="N177" t="inlineStr"/>
+      <c r="N177" t="n">
+        <v>0</v>
+      </c>
       <c r="O177" t="n">
         <v>20</v>
       </c>
@@ -20516,7 +20868,9 @@
       <c r="M178" t="n">
         <v>3800</v>
       </c>
-      <c r="N178" t="inlineStr"/>
+      <c r="N178" t="n">
+        <v>0</v>
+      </c>
       <c r="O178" t="n">
         <v>20</v>
       </c>
@@ -20630,7 +20984,9 @@
       <c r="M179" t="n">
         <v>4400</v>
       </c>
-      <c r="N179" t="inlineStr"/>
+      <c r="N179" t="n">
+        <v>0</v>
+      </c>
       <c r="O179" t="n">
         <v>20</v>
       </c>
@@ -20744,7 +21100,9 @@
       <c r="M180" t="n">
         <v>18000</v>
       </c>
-      <c r="N180" t="inlineStr"/>
+      <c r="N180" t="n">
+        <v>0</v>
+      </c>
       <c r="O180" t="n">
         <v>20</v>
       </c>
@@ -20858,7 +21216,9 @@
       <c r="M181" t="n">
         <v>19170</v>
       </c>
-      <c r="N181" t="inlineStr"/>
+      <c r="N181" t="n">
+        <v>0</v>
+      </c>
       <c r="O181" t="n">
         <v>20</v>
       </c>
@@ -20972,7 +21332,9 @@
       <c r="M182" t="n">
         <v>1625</v>
       </c>
-      <c r="N182" t="inlineStr"/>
+      <c r="N182" t="n">
+        <v>0</v>
+      </c>
       <c r="O182" t="n">
         <v>20</v>
       </c>
@@ -21086,7 +21448,9 @@
       <c r="M183" t="n">
         <v>3575</v>
       </c>
-      <c r="N183" t="inlineStr"/>
+      <c r="N183" t="n">
+        <v>0</v>
+      </c>
       <c r="O183" t="n">
         <v>20</v>
       </c>
@@ -21201,7 +21565,9 @@
       <c r="M184" t="n">
         <v>4550</v>
       </c>
-      <c r="N184" t="inlineStr"/>
+      <c r="N184" t="n">
+        <v>0</v>
+      </c>
       <c r="O184" t="n">
         <v>20</v>
       </c>
@@ -21315,7 +21681,9 @@
       <c r="M185" t="n">
         <v>1755</v>
       </c>
-      <c r="N185" t="inlineStr"/>
+      <c r="N185" t="n">
+        <v>0</v>
+      </c>
       <c r="O185" t="n">
         <v>20</v>
       </c>
@@ -21429,7 +21797,9 @@
       <c r="M186" t="n">
         <v>7000</v>
       </c>
-      <c r="N186" t="inlineStr"/>
+      <c r="N186" t="n">
+        <v>0</v>
+      </c>
       <c r="O186" t="n">
         <v>20</v>
       </c>
@@ -21543,7 +21913,9 @@
       <c r="M187" t="n">
         <v>420</v>
       </c>
-      <c r="N187" t="inlineStr"/>
+      <c r="N187" t="n">
+        <v>0</v>
+      </c>
       <c r="O187" t="n">
         <v>20</v>
       </c>
@@ -21657,7 +22029,9 @@
       <c r="M188" t="n">
         <v>3780</v>
       </c>
-      <c r="N188" t="inlineStr"/>
+      <c r="N188" t="n">
+        <v>0</v>
+      </c>
       <c r="O188" t="n">
         <v>20</v>
       </c>
@@ -21771,7 +22145,9 @@
       <c r="M189" t="n">
         <v>125000</v>
       </c>
-      <c r="N189" t="inlineStr"/>
+      <c r="N189" t="n">
+        <v>0</v>
+      </c>
       <c r="O189" t="n">
         <v>20</v>
       </c>
@@ -21885,7 +22261,9 @@
       <c r="M190" t="n">
         <v>24900</v>
       </c>
-      <c r="N190" t="inlineStr"/>
+      <c r="N190" t="n">
+        <v>0</v>
+      </c>
       <c r="O190" t="n">
         <v>20</v>
       </c>
@@ -21999,7 +22377,9 @@
       <c r="M191" t="n">
         <v>6500</v>
       </c>
-      <c r="N191" t="inlineStr"/>
+      <c r="N191" t="n">
+        <v>0</v>
+      </c>
       <c r="O191" t="n">
         <v>20</v>
       </c>
@@ -22113,7 +22493,9 @@
       <c r="M192" t="n">
         <v>3750</v>
       </c>
-      <c r="N192" t="inlineStr"/>
+      <c r="N192" t="n">
+        <v>0</v>
+      </c>
       <c r="O192" t="n">
         <v>20</v>
       </c>
@@ -22227,7 +22609,9 @@
       <c r="M193" t="n">
         <v>11100</v>
       </c>
-      <c r="N193" t="inlineStr"/>
+      <c r="N193" t="n">
+        <v>0</v>
+      </c>
       <c r="O193" t="n">
         <v>15</v>
       </c>
@@ -22341,7 +22725,9 @@
       <c r="M194" t="n">
         <v>29900</v>
       </c>
-      <c r="N194" t="inlineStr"/>
+      <c r="N194" t="n">
+        <v>0</v>
+      </c>
       <c r="O194" t="n">
         <v>15</v>
       </c>
@@ -22455,7 +22841,9 @@
       <c r="M195" t="n">
         <v>6250</v>
       </c>
-      <c r="N195" t="inlineStr"/>
+      <c r="N195" t="n">
+        <v>0</v>
+      </c>
       <c r="O195" t="n">
         <v>15</v>
       </c>
@@ -22569,7 +22957,9 @@
       <c r="M196" t="n">
         <v>12150</v>
       </c>
-      <c r="N196" t="inlineStr"/>
+      <c r="N196" t="n">
+        <v>0</v>
+      </c>
       <c r="O196" t="n">
         <v>15</v>
       </c>
@@ -22683,7 +23073,9 @@
       <c r="M197" t="n">
         <v>7500</v>
       </c>
-      <c r="N197" t="inlineStr"/>
+      <c r="N197" t="n">
+        <v>0</v>
+      </c>
       <c r="O197" t="n">
         <v>15</v>
       </c>
@@ -22797,7 +23189,9 @@
       <c r="M198" t="n">
         <v>2625</v>
       </c>
-      <c r="N198" t="inlineStr"/>
+      <c r="N198" t="n">
+        <v>0</v>
+      </c>
       <c r="O198" t="n">
         <v>15</v>
       </c>
@@ -22911,7 +23305,9 @@
       <c r="M199" t="n">
         <v>18375</v>
       </c>
-      <c r="N199" t="inlineStr"/>
+      <c r="N199" t="n">
+        <v>0</v>
+      </c>
       <c r="O199" t="n">
         <v>15</v>
       </c>
@@ -23025,7 +23421,9 @@
       <c r="M200" t="n">
         <v>3360</v>
       </c>
-      <c r="N200" t="inlineStr"/>
+      <c r="N200" t="n">
+        <v>0</v>
+      </c>
       <c r="O200" t="n">
         <v>15</v>
       </c>
@@ -23139,7 +23537,9 @@
       <c r="M201" t="n">
         <v>2062.5</v>
       </c>
-      <c r="N201" t="inlineStr"/>
+      <c r="N201" t="n">
+        <v>0</v>
+      </c>
       <c r="O201" t="n">
         <v>15</v>
       </c>
@@ -23253,7 +23653,9 @@
       <c r="M202" t="n">
         <v>13125</v>
       </c>
-      <c r="N202" t="inlineStr"/>
+      <c r="N202" t="n">
+        <v>0</v>
+      </c>
       <c r="O202" t="n">
         <v>15</v>
       </c>
@@ -23367,7 +23769,9 @@
       <c r="M203" t="n">
         <v>2100</v>
       </c>
-      <c r="N203" t="inlineStr"/>
+      <c r="N203" t="n">
+        <v>0</v>
+      </c>
       <c r="O203" t="n">
         <v>15</v>
       </c>
@@ -23481,7 +23885,9 @@
       <c r="M204" t="n">
         <v>86100</v>
       </c>
-      <c r="N204" t="inlineStr"/>
+      <c r="N204" t="n">
+        <v>0</v>
+      </c>
       <c r="O204" t="n">
         <v>15</v>
       </c>
@@ -23595,7 +24001,9 @@
       <c r="M205" t="n">
         <v>196500</v>
       </c>
-      <c r="N205" t="inlineStr"/>
+      <c r="N205" t="n">
+        <v>0</v>
+      </c>
       <c r="O205" t="n">
         <v>15</v>
       </c>
@@ -23709,7 +24117,9 @@
       <c r="M206" t="n">
         <v>1560</v>
       </c>
-      <c r="N206" t="inlineStr"/>
+      <c r="N206" t="n">
+        <v>0</v>
+      </c>
       <c r="O206" t="n">
         <v>15</v>
       </c>
@@ -23823,7 +24233,9 @@
       <c r="M207" t="n">
         <v>22340</v>
       </c>
-      <c r="N207" t="inlineStr"/>
+      <c r="N207" t="n">
+        <v>0</v>
+      </c>
       <c r="O207" t="n">
         <v>15</v>
       </c>
@@ -23937,7 +24349,9 @@
       <c r="M208" t="n">
         <v>52360</v>
       </c>
-      <c r="N208" t="inlineStr"/>
+      <c r="N208" t="n">
+        <v>0</v>
+      </c>
       <c r="O208" t="n">
         <v>15</v>
       </c>
@@ -24051,7 +24465,9 @@
       <c r="M209" t="n">
         <v>11875</v>
       </c>
-      <c r="N209" t="inlineStr"/>
+      <c r="N209" t="n">
+        <v>0</v>
+      </c>
       <c r="O209" t="n">
         <v>15</v>
       </c>
@@ -24165,7 +24581,9 @@
       <c r="M210" t="n">
         <v>15675</v>
       </c>
-      <c r="N210" t="inlineStr"/>
+      <c r="N210" t="n">
+        <v>0</v>
+      </c>
       <c r="O210" t="n">
         <v>15</v>
       </c>
@@ -24279,7 +24697,9 @@
       <c r="M211" t="n">
         <v>3000</v>
       </c>
-      <c r="N211" t="inlineStr"/>
+      <c r="N211" t="n">
+        <v>0</v>
+      </c>
       <c r="O211" t="n">
         <v>15</v>
       </c>
@@ -24393,7 +24813,9 @@
       <c r="M212" t="n">
         <v>6030</v>
       </c>
-      <c r="N212" t="inlineStr"/>
+      <c r="N212" t="n">
+        <v>0</v>
+      </c>
       <c r="O212" t="n">
         <v>15</v>
       </c>
@@ -24507,7 +24929,9 @@
       <c r="M213" t="n">
         <v>8250</v>
       </c>
-      <c r="N213" t="inlineStr"/>
+      <c r="N213" t="n">
+        <v>0</v>
+      </c>
       <c r="O213" t="n">
         <v>15</v>
       </c>
@@ -24621,7 +25045,9 @@
       <c r="M214" t="n">
         <v>1950</v>
       </c>
-      <c r="N214" t="inlineStr"/>
+      <c r="N214" t="n">
+        <v>0</v>
+      </c>
       <c r="O214" t="n">
         <v>15</v>
       </c>
@@ -24735,7 +25161,9 @@
       <c r="M215" t="n">
         <v>23200</v>
       </c>
-      <c r="N215" t="inlineStr"/>
+      <c r="N215" t="n">
+        <v>0</v>
+      </c>
       <c r="O215" t="n">
         <v>15</v>
       </c>
@@ -24849,7 +25277,9 @@
       <c r="M216" t="n">
         <v>3500</v>
       </c>
-      <c r="N216" t="inlineStr"/>
+      <c r="N216" t="n">
+        <v>0</v>
+      </c>
       <c r="O216" t="n">
         <v>15</v>
       </c>
@@ -24963,7 +25393,9 @@
       <c r="M217" t="n">
         <v>78750</v>
       </c>
-      <c r="N217" t="inlineStr"/>
+      <c r="N217" t="n">
+        <v>0</v>
+      </c>
       <c r="O217" t="n">
         <v>15</v>
       </c>
@@ -25077,7 +25509,9 @@
       <c r="M218" t="n">
         <v>175000</v>
       </c>
-      <c r="N218" t="inlineStr"/>
+      <c r="N218" t="n">
+        <v>0</v>
+      </c>
       <c r="O218" t="n">
         <v>15</v>
       </c>
@@ -25191,7 +25625,9 @@
       <c r="M219" t="n">
         <v>97500</v>
       </c>
-      <c r="N219" t="inlineStr"/>
+      <c r="N219" t="n">
+        <v>0</v>
+      </c>
       <c r="O219" t="n">
         <v>15</v>
       </c>
@@ -25305,7 +25741,9 @@
       <c r="M220" t="n">
         <v>30500</v>
       </c>
-      <c r="N220" t="inlineStr"/>
+      <c r="N220" t="n">
+        <v>0</v>
+      </c>
       <c r="O220" t="n">
         <v>15</v>
       </c>
@@ -25419,7 +25857,9 @@
       <c r="M221" t="n">
         <v>15000</v>
       </c>
-      <c r="N221" t="inlineStr"/>
+      <c r="N221" t="n">
+        <v>0</v>
+      </c>
       <c r="O221" t="n">
         <v>15</v>
       </c>
@@ -25533,7 +25973,9 @@
       <c r="M222" t="n">
         <v>12825</v>
       </c>
-      <c r="N222" t="inlineStr"/>
+      <c r="N222" t="n">
+        <v>0</v>
+      </c>
       <c r="O222" t="n">
         <v>15</v>
       </c>
@@ -25647,7 +26089,9 @@
       <c r="M223" t="n">
         <v>43875</v>
       </c>
-      <c r="N223" t="inlineStr"/>
+      <c r="N223" t="n">
+        <v>0</v>
+      </c>
       <c r="O223" t="n">
         <v>15</v>
       </c>
@@ -25761,7 +26205,9 @@
       <c r="M224" t="n">
         <v>30600</v>
       </c>
-      <c r="N224" t="inlineStr"/>
+      <c r="N224" t="n">
+        <v>0</v>
+      </c>
       <c r="O224" t="n">
         <v>15</v>
       </c>
@@ -25875,7 +26321,9 @@
       <c r="M225" t="n">
         <v>4143.75</v>
       </c>
-      <c r="N225" t="inlineStr"/>
+      <c r="N225" t="n">
+        <v>0</v>
+      </c>
       <c r="O225" t="n">
         <v>15</v>
       </c>
@@ -25989,7 +26437,9 @@
       <c r="M226" t="n">
         <v>81375</v>
       </c>
-      <c r="N226" t="inlineStr"/>
+      <c r="N226" t="n">
+        <v>0</v>
+      </c>
       <c r="O226" t="n">
         <v>15</v>
       </c>
@@ -26103,7 +26553,9 @@
       <c r="M227" t="n">
         <v>107000</v>
       </c>
-      <c r="N227" t="inlineStr"/>
+      <c r="N227" t="n">
+        <v>0</v>
+      </c>
       <c r="O227" t="n">
         <v>15</v>
       </c>
@@ -26217,7 +26669,9 @@
       <c r="M228" t="n">
         <v>16575</v>
       </c>
-      <c r="N228" t="inlineStr"/>
+      <c r="N228" t="n">
+        <v>0</v>
+      </c>
       <c r="O228" t="n">
         <v>15</v>
       </c>
@@ -26331,7 +26785,9 @@
       <c r="M229" t="n">
         <v>22000</v>
       </c>
-      <c r="N229" t="inlineStr"/>
+      <c r="N229" t="n">
+        <v>0</v>
+      </c>
       <c r="O229" t="n">
         <v>15</v>
       </c>
@@ -26445,7 +26901,9 @@
       <c r="M230" t="n">
         <v>14700</v>
       </c>
-      <c r="N230" t="inlineStr"/>
+      <c r="N230" t="n">
+        <v>0</v>
+      </c>
       <c r="O230" t="n">
         <v>15</v>
       </c>
@@ -26559,7 +27017,9 @@
       <c r="M231" t="n">
         <v>715</v>
       </c>
-      <c r="N231" t="inlineStr"/>
+      <c r="N231" t="n">
+        <v>0</v>
+      </c>
       <c r="O231" t="n">
         <v>15</v>
       </c>
@@ -26673,7 +27133,9 @@
       <c r="M232" t="n">
         <v>3895</v>
       </c>
-      <c r="N232" t="inlineStr"/>
+      <c r="N232" t="n">
+        <v>0</v>
+      </c>
       <c r="O232" t="n">
         <v>15</v>
       </c>
@@ -26787,7 +27249,9 @@
       <c r="M233" t="n">
         <v>57150</v>
       </c>
-      <c r="N233" t="inlineStr"/>
+      <c r="N233" t="n">
+        <v>0</v>
+      </c>
       <c r="O233" t="n">
         <v>15</v>
       </c>
@@ -26901,7 +27365,9 @@
       <c r="M234" t="n">
         <v>12750</v>
       </c>
-      <c r="N234" t="inlineStr"/>
+      <c r="N234" t="n">
+        <v>0</v>
+      </c>
       <c r="O234" t="n">
         <v>15</v>
       </c>
@@ -27015,7 +27481,9 @@
       <c r="M235" t="n">
         <v>90000</v>
       </c>
-      <c r="N235" t="inlineStr"/>
+      <c r="N235" t="n">
+        <v>0</v>
+      </c>
       <c r="O235" t="n">
         <v>15</v>
       </c>
@@ -27129,7 +27597,9 @@
       <c r="M236" t="n">
         <v>34500</v>
       </c>
-      <c r="N236" t="inlineStr"/>
+      <c r="N236" t="n">
+        <v>0</v>
+      </c>
       <c r="O236" t="n">
         <v>15</v>
       </c>
@@ -27243,7 +27713,9 @@
       <c r="M237" t="n">
         <v>226248.75</v>
       </c>
-      <c r="N237" t="inlineStr"/>
+      <c r="N237" t="n">
+        <v>0</v>
+      </c>
       <c r="O237" t="n">
         <v>10</v>
       </c>
@@ -27357,7 +27829,9 @@
       <c r="M238" t="n">
         <v>42525</v>
       </c>
-      <c r="N238" t="inlineStr"/>
+      <c r="N238" t="n">
+        <v>0</v>
+      </c>
       <c r="O238" t="n">
         <v>10</v>
       </c>
@@ -27471,7 +27945,9 @@
       <c r="M239" t="n">
         <v>29250</v>
       </c>
-      <c r="N239" t="inlineStr"/>
+      <c r="N239" t="n">
+        <v>0</v>
+      </c>
       <c r="O239" t="n">
         <v>10</v>
       </c>
@@ -27585,7 +28061,9 @@
       <c r="M240" t="n">
         <v>55560</v>
       </c>
-      <c r="N240" t="inlineStr"/>
+      <c r="N240" t="n">
+        <v>0</v>
+      </c>
       <c r="O240" t="n">
         <v>10</v>
       </c>
@@ -27699,7 +28177,9 @@
       <c r="M241" t="n">
         <v>22385</v>
       </c>
-      <c r="N241" t="inlineStr"/>
+      <c r="N241" t="n">
+        <v>0</v>
+      </c>
       <c r="O241" t="n">
         <v>10</v>
       </c>
@@ -27813,7 +28293,9 @@
       <c r="M242" t="n">
         <v>57701.1</v>
       </c>
-      <c r="N242" t="inlineStr"/>
+      <c r="N242" t="n">
+        <v>0</v>
+      </c>
       <c r="O242" t="n">
         <v>20</v>
       </c>
@@ -27927,7 +28409,9 @@
       <c r="M243" t="n">
         <v>235951.5</v>
       </c>
-      <c r="N243" t="inlineStr"/>
+      <c r="N243" t="n">
+        <v>0</v>
+      </c>
       <c r="O243" t="n">
         <v>20</v>
       </c>
@@ -28041,7 +28525,9 @@
       <c r="M244" t="n">
         <v>141805.5</v>
       </c>
-      <c r="N244" t="inlineStr"/>
+      <c r="N244" t="n">
+        <v>0</v>
+      </c>
       <c r="O244" t="n">
         <v>20</v>
       </c>
@@ -28155,7 +28641,9 @@
       <c r="M245" t="n">
         <v>211901.7</v>
       </c>
-      <c r="N245" t="inlineStr"/>
+      <c r="N245" t="n">
+        <v>0</v>
+      </c>
       <c r="O245" t="n">
         <v>20</v>
       </c>
@@ -28269,7 +28757,9 @@
       <c r="M246" t="n">
         <v>103382.4</v>
       </c>
-      <c r="N246" t="inlineStr"/>
+      <c r="N246" t="n">
+        <v>0</v>
+      </c>
       <c r="O246" t="n">
         <v>20</v>
       </c>
@@ -28383,7 +28873,9 @@
       <c r="M247" t="n">
         <v>270286.8</v>
       </c>
-      <c r="N247" t="inlineStr"/>
+      <c r="N247" t="n">
+        <v>0</v>
+      </c>
       <c r="O247" t="n">
         <v>20</v>
       </c>
@@ -28497,7 +28989,9 @@
       <c r="M248" t="n">
         <v>58650</v>
       </c>
-      <c r="N248" t="inlineStr"/>
+      <c r="N248" t="n">
+        <v>0</v>
+      </c>
       <c r="O248" t="n">
         <v>20</v>
       </c>
@@ -28611,7 +29105,9 @@
       <c r="M249" t="n">
         <v>3000</v>
       </c>
-      <c r="N249" t="inlineStr"/>
+      <c r="N249" t="n">
+        <v>0</v>
+      </c>
       <c r="O249" t="n">
         <v>20</v>
       </c>
@@ -28725,7 +29221,9 @@
       <c r="M250" t="n">
         <v>115152.45</v>
       </c>
-      <c r="N250" t="inlineStr"/>
+      <c r="N250" t="n">
+        <v>0</v>
+      </c>
       <c r="O250" t="n">
         <v>20</v>
       </c>
@@ -28839,7 +29337,9 @@
       <c r="M251" t="n">
         <v>52387.5</v>
       </c>
-      <c r="N251" t="inlineStr"/>
+      <c r="N251" t="n">
+        <v>0</v>
+      </c>
       <c r="O251" t="n">
         <v>20</v>
       </c>
@@ -28953,7 +29453,9 @@
       <c r="M252" t="n">
         <v>28500</v>
       </c>
-      <c r="N252" t="inlineStr"/>
+      <c r="N252" t="n">
+        <v>0</v>
+      </c>
       <c r="O252" t="n">
         <v>20</v>
       </c>
@@ -29067,7 +29569,9 @@
       <c r="M253" t="n">
         <v>69080</v>
       </c>
-      <c r="N253" t="inlineStr"/>
+      <c r="N253" t="n">
+        <v>0</v>
+      </c>
       <c r="O253" t="n">
         <v>20</v>
       </c>
@@ -29181,7 +29685,9 @@
       <c r="M254" t="n">
         <v>708513</v>
       </c>
-      <c r="N254" t="inlineStr"/>
+      <c r="N254" t="n">
+        <v>0</v>
+      </c>
       <c r="O254" t="n">
         <v>20</v>
       </c>
@@ -29295,7 +29801,9 @@
       <c r="M255" t="n">
         <v>480000</v>
       </c>
-      <c r="N255" t="inlineStr"/>
+      <c r="N255" t="n">
+        <v>0</v>
+      </c>
       <c r="O255" t="n">
         <v>20</v>
       </c>
@@ -29409,7 +29917,9 @@
       <c r="M256" t="n">
         <v>596805</v>
       </c>
-      <c r="N256" t="inlineStr"/>
+      <c r="N256" t="n">
+        <v>0</v>
+      </c>
       <c r="O256" t="n">
         <v>20</v>
       </c>
@@ -29523,7 +30033,9 @@
       <c r="M257" t="n">
         <v>43112.85</v>
       </c>
-      <c r="N257" t="inlineStr"/>
+      <c r="N257" t="n">
+        <v>0</v>
+      </c>
       <c r="O257" t="n">
         <v>20</v>
       </c>
@@ -29637,7 +30149,9 @@
       <c r="M258" t="n">
         <v>109200</v>
       </c>
-      <c r="N258" t="inlineStr"/>
+      <c r="N258" t="n">
+        <v>0</v>
+      </c>
       <c r="O258" t="n">
         <v>20</v>
       </c>
@@ -29751,7 +30265,9 @@
       <c r="M259" t="n">
         <v>39375</v>
       </c>
-      <c r="N259" t="inlineStr"/>
+      <c r="N259" t="n">
+        <v>0</v>
+      </c>
       <c r="O259" t="n">
         <v>20</v>
       </c>
@@ -29865,7 +30381,9 @@
       <c r="M260" t="n">
         <v>110250</v>
       </c>
-      <c r="N260" t="inlineStr"/>
+      <c r="N260" t="n">
+        <v>0</v>
+      </c>
       <c r="O260" t="n">
         <v>20</v>
       </c>
@@ -29979,7 +30497,9 @@
       <c r="M261" t="n">
         <v>215845.5</v>
       </c>
-      <c r="N261" t="inlineStr"/>
+      <c r="N261" t="n">
+        <v>0</v>
+      </c>
       <c r="O261" t="n">
         <v>20</v>
       </c>
@@ -30093,7 +30613,9 @@
       <c r="M262" t="n">
         <v>36387.75</v>
       </c>
-      <c r="N262" t="inlineStr"/>
+      <c r="N262" t="n">
+        <v>0</v>
+      </c>
       <c r="O262" t="n">
         <v>20</v>
       </c>
@@ -30207,7 +30729,9 @@
       <c r="M263" t="n">
         <v>86708.39999999999</v>
       </c>
-      <c r="N263" t="inlineStr"/>
+      <c r="N263" t="n">
+        <v>0</v>
+      </c>
       <c r="O263" t="n">
         <v>20</v>
       </c>
@@ -30321,7 +30845,9 @@
       <c r="M264" t="n">
         <v>250930.35</v>
       </c>
-      <c r="N264" t="inlineStr"/>
+      <c r="N264" t="n">
+        <v>0</v>
+      </c>
       <c r="O264" t="n">
         <v>20</v>
       </c>
@@ -30435,7 +30961,9 @@
       <c r="M265" t="n">
         <v>37275</v>
       </c>
-      <c r="N265" t="inlineStr"/>
+      <c r="N265" t="n">
+        <v>0</v>
+      </c>
       <c r="O265" t="n">
         <v>20</v>
       </c>
@@ -30549,7 +31077,9 @@
       <c r="M266" t="n">
         <v>31674</v>
       </c>
-      <c r="N266" t="inlineStr"/>
+      <c r="N266" t="n">
+        <v>0</v>
+      </c>
       <c r="O266" t="n">
         <v>20</v>
       </c>
@@ -30663,7 +31193,9 @@
       <c r="M267" t="n">
         <v>21500</v>
       </c>
-      <c r="N267" t="inlineStr"/>
+      <c r="N267" t="n">
+        <v>0</v>
+      </c>
       <c r="O267" t="n">
         <v>20</v>
       </c>
@@ -30777,7 +31309,9 @@
       <c r="M268" t="n">
         <v>145000</v>
       </c>
-      <c r="N268" t="inlineStr"/>
+      <c r="N268" t="n">
+        <v>0</v>
+      </c>
       <c r="O268" t="n">
         <v>20</v>
       </c>
@@ -30891,7 +31425,9 @@
       <c r="M269" t="n">
         <v>36267.2</v>
       </c>
-      <c r="N269" t="inlineStr"/>
+      <c r="N269" t="n">
+        <v>0</v>
+      </c>
       <c r="O269" t="n">
         <v>20</v>
       </c>
@@ -31005,7 +31541,9 @@
       <c r="M270" t="n">
         <v>83200</v>
       </c>
-      <c r="N270" t="inlineStr"/>
+      <c r="N270" t="n">
+        <v>0</v>
+      </c>
       <c r="O270" t="n">
         <v>20</v>
       </c>
@@ -31119,7 +31657,9 @@
       <c r="M271" t="n">
         <v>74750</v>
       </c>
-      <c r="N271" t="inlineStr"/>
+      <c r="N271" t="n">
+        <v>0</v>
+      </c>
       <c r="O271" t="n">
         <v>20</v>
       </c>
@@ -31233,7 +31773,9 @@
       <c r="M272" t="n">
         <v>140600</v>
       </c>
-      <c r="N272" t="inlineStr"/>
+      <c r="N272" t="n">
+        <v>0</v>
+      </c>
       <c r="O272" t="n">
         <v>20</v>
       </c>
@@ -31347,7 +31889,9 @@
       <c r="M273" t="n">
         <v>134186.25</v>
       </c>
-      <c r="N273" t="inlineStr"/>
+      <c r="N273" t="n">
+        <v>0</v>
+      </c>
       <c r="O273" t="n">
         <v>20</v>
       </c>
@@ -31461,7 +32005,9 @@
       <c r="M274" t="n">
         <v>3900</v>
       </c>
-      <c r="N274" t="inlineStr"/>
+      <c r="N274" t="n">
+        <v>0</v>
+      </c>
       <c r="O274" t="n">
         <v>20</v>
       </c>
@@ -31575,7 +32121,9 @@
       <c r="M275" t="n">
         <v>1000000</v>
       </c>
-      <c r="N275" t="inlineStr"/>
+      <c r="N275" t="n">
+        <v>0</v>
+      </c>
       <c r="O275" t="n">
         <v>15</v>
       </c>
@@ -31689,7 +32237,9 @@
       <c r="M276" t="n">
         <v>117000</v>
       </c>
-      <c r="N276" t="inlineStr"/>
+      <c r="N276" t="n">
+        <v>0</v>
+      </c>
       <c r="O276" t="n">
         <v>15</v>
       </c>
@@ -31803,7 +32353,9 @@
       <c r="M277" t="n">
         <v>165000</v>
       </c>
-      <c r="N277" t="inlineStr"/>
+      <c r="N277" t="n">
+        <v>0</v>
+      </c>
       <c r="O277" t="n">
         <v>15</v>
       </c>
@@ -31917,7 +32469,9 @@
       <c r="M278" t="n">
         <v>47500</v>
       </c>
-      <c r="N278" t="inlineStr"/>
+      <c r="N278" t="n">
+        <v>0</v>
+      </c>
       <c r="O278" t="n">
         <v>15</v>
       </c>
@@ -32031,7 +32585,9 @@
       <c r="M279" t="n">
         <v>73500</v>
       </c>
-      <c r="N279" t="inlineStr"/>
+      <c r="N279" t="n">
+        <v>0</v>
+      </c>
       <c r="O279" t="n">
         <v>15</v>
       </c>
@@ -32145,7 +32701,9 @@
       <c r="M280" t="n">
         <v>50800</v>
       </c>
-      <c r="N280" t="inlineStr"/>
+      <c r="N280" t="n">
+        <v>0</v>
+      </c>
       <c r="O280" t="n">
         <v>15</v>
       </c>
@@ -32259,7 +32817,9 @@
       <c r="M281" t="n">
         <v>47000</v>
       </c>
-      <c r="N281" t="inlineStr"/>
+      <c r="N281" t="n">
+        <v>0</v>
+      </c>
       <c r="O281" t="n">
         <v>15</v>
       </c>
@@ -32373,7 +32933,9 @@
       <c r="M282" t="n">
         <v>96000</v>
       </c>
-      <c r="N282" t="inlineStr"/>
+      <c r="N282" t="n">
+        <v>0</v>
+      </c>
       <c r="O282" t="n">
         <v>15</v>
       </c>
@@ -32487,7 +33049,9 @@
       <c r="M283" t="n">
         <v>220800</v>
       </c>
-      <c r="N283" t="inlineStr"/>
+      <c r="N283" t="n">
+        <v>0</v>
+      </c>
       <c r="O283" t="n">
         <v>15</v>
       </c>
@@ -32601,7 +33165,9 @@
       <c r="M284" t="n">
         <v>65000</v>
       </c>
-      <c r="N284" t="inlineStr"/>
+      <c r="N284" t="n">
+        <v>0</v>
+      </c>
       <c r="O284" t="n">
         <v>15</v>
       </c>
@@ -32715,7 +33281,9 @@
       <c r="M285" t="n">
         <v>87000</v>
       </c>
-      <c r="N285" t="inlineStr"/>
+      <c r="N285" t="n">
+        <v>0</v>
+      </c>
       <c r="O285" t="n">
         <v>15</v>
       </c>
@@ -32829,7 +33397,9 @@
       <c r="M286" t="n">
         <v>140000</v>
       </c>
-      <c r="N286" t="inlineStr"/>
+      <c r="N286" t="n">
+        <v>0</v>
+      </c>
       <c r="O286" t="n">
         <v>15</v>
       </c>
@@ -32943,7 +33513,9 @@
       <c r="M287" t="n">
         <v>95000</v>
       </c>
-      <c r="N287" t="inlineStr"/>
+      <c r="N287" t="n">
+        <v>0</v>
+      </c>
       <c r="O287" t="n">
         <v>15</v>
       </c>
@@ -33057,7 +33629,9 @@
       <c r="M288" t="n">
         <v>60000</v>
       </c>
-      <c r="N288" t="inlineStr"/>
+      <c r="N288" t="n">
+        <v>0</v>
+      </c>
       <c r="O288" t="n">
         <v>15</v>
       </c>
@@ -33171,7 +33745,9 @@
       <c r="M289" t="n">
         <v>422500</v>
       </c>
-      <c r="N289" t="inlineStr"/>
+      <c r="N289" t="n">
+        <v>0</v>
+      </c>
       <c r="O289" t="n">
         <v>15</v>
       </c>
@@ -33285,7 +33861,9 @@
       <c r="M290" t="n">
         <v>8450</v>
       </c>
-      <c r="N290" t="inlineStr"/>
+      <c r="N290" t="n">
+        <v>0</v>
+      </c>
       <c r="O290" t="n">
         <v>15</v>
       </c>
@@ -33399,7 +33977,9 @@
       <c r="M291" t="n">
         <v>60000</v>
       </c>
-      <c r="N291" t="inlineStr"/>
+      <c r="N291" t="n">
+        <v>0</v>
+      </c>
       <c r="O291" t="n">
         <v>15</v>
       </c>
@@ -33513,7 +34093,9 @@
       <c r="M292" t="n">
         <v>23400</v>
       </c>
-      <c r="N292" t="inlineStr"/>
+      <c r="N292" t="n">
+        <v>0</v>
+      </c>
       <c r="O292" t="n">
         <v>15</v>
       </c>
@@ -33627,7 +34209,9 @@
       <c r="M293" t="n">
         <v>118430</v>
       </c>
-      <c r="N293" t="inlineStr"/>
+      <c r="N293" t="n">
+        <v>0</v>
+      </c>
       <c r="O293" t="n">
         <v>15</v>
       </c>
@@ -33741,7 +34325,9 @@
       <c r="M294" t="n">
         <v>8937.5</v>
       </c>
-      <c r="N294" t="inlineStr"/>
+      <c r="N294" t="n">
+        <v>0</v>
+      </c>
       <c r="O294" t="n">
         <v>15</v>
       </c>
@@ -33855,7 +34441,9 @@
       <c r="M295" t="n">
         <v>200000</v>
       </c>
-      <c r="N295" t="inlineStr"/>
+      <c r="N295" t="n">
+        <v>0</v>
+      </c>
       <c r="O295" t="n">
         <v>15</v>
       </c>
@@ -33969,7 +34557,9 @@
       <c r="M296" t="n">
         <v>1182360</v>
       </c>
-      <c r="N296" t="inlineStr"/>
+      <c r="N296" t="n">
+        <v>0</v>
+      </c>
       <c r="O296" t="n">
         <v>15</v>
       </c>
@@ -34083,7 +34673,9 @@
       <c r="M297" t="n">
         <v>120000</v>
       </c>
-      <c r="N297" t="inlineStr"/>
+      <c r="N297" t="n">
+        <v>0</v>
+      </c>
       <c r="O297" t="n">
         <v>15</v>
       </c>
@@ -34197,7 +34789,9 @@
       <c r="M298" t="n">
         <v>78800</v>
       </c>
-      <c r="N298" t="inlineStr"/>
+      <c r="N298" t="n">
+        <v>0</v>
+      </c>
       <c r="O298" t="n">
         <v>15</v>
       </c>
@@ -34311,7 +34905,9 @@
       <c r="M299" t="n">
         <v>50100</v>
       </c>
-      <c r="N299" t="inlineStr"/>
+      <c r="N299" t="n">
+        <v>0</v>
+      </c>
       <c r="O299" t="n">
         <v>15</v>
       </c>
@@ -34425,7 +35021,9 @@
       <c r="M300" t="n">
         <v>188000</v>
       </c>
-      <c r="N300" t="inlineStr"/>
+      <c r="N300" t="n">
+        <v>0</v>
+      </c>
       <c r="O300" t="n">
         <v>15</v>
       </c>
@@ -34539,7 +35137,9 @@
       <c r="M301" t="n">
         <v>45500</v>
       </c>
-      <c r="N301" t="inlineStr"/>
+      <c r="N301" t="n">
+        <v>0</v>
+      </c>
       <c r="O301" t="n">
         <v>15</v>
       </c>
@@ -34651,7 +35251,9 @@
       <c r="M302" t="n">
         <v>2132</v>
       </c>
-      <c r="N302" t="inlineStr"/>
+      <c r="N302" t="n">
+        <v>0</v>
+      </c>
       <c r="O302" t="n">
         <v>10</v>
       </c>
@@ -34660,7 +35262,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q302" t="inlineStr"/>
+      <c r="Q302" t="n">
+        <v>0</v>
+      </c>
       <c r="R302" t="n">
         <v>0</v>
       </c>
@@ -34676,9 +35280,15 @@
       <c r="V302" t="n">
         <v>426.4</v>
       </c>
-      <c r="W302" t="inlineStr"/>
-      <c r="X302" t="inlineStr"/>
-      <c r="Y302" t="inlineStr"/>
+      <c r="W302" t="n">
+        <v>0</v>
+      </c>
+      <c r="X302" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y302" t="n">
+        <v>0</v>
+      </c>
       <c r="Z302" t="n">
         <v>0</v>
       </c>
@@ -34757,7 +35367,9 @@
       <c r="M303" t="n">
         <v>2132</v>
       </c>
-      <c r="N303" t="inlineStr"/>
+      <c r="N303" t="n">
+        <v>0</v>
+      </c>
       <c r="O303" t="n">
         <v>10</v>
       </c>
@@ -34766,7 +35378,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q303" t="inlineStr"/>
+      <c r="Q303" t="n">
+        <v>0</v>
+      </c>
       <c r="R303" t="n">
         <v>0</v>
       </c>
@@ -34782,9 +35396,15 @@
       <c r="V303" t="n">
         <v>426.4</v>
       </c>
-      <c r="W303" t="inlineStr"/>
-      <c r="X303" t="inlineStr"/>
-      <c r="Y303" t="inlineStr"/>
+      <c r="W303" t="n">
+        <v>0</v>
+      </c>
+      <c r="X303" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y303" t="n">
+        <v>0</v>
+      </c>
       <c r="Z303" t="n">
         <v>0</v>
       </c>
@@ -34863,7 +35483,9 @@
       <c r="M304" t="n">
         <v>2112</v>
       </c>
-      <c r="N304" t="inlineStr"/>
+      <c r="N304" t="n">
+        <v>0</v>
+      </c>
       <c r="O304" t="n">
         <v>10</v>
       </c>
@@ -34872,7 +35494,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q304" t="inlineStr"/>
+      <c r="Q304" t="n">
+        <v>0</v>
+      </c>
       <c r="R304" t="n">
         <v>0</v>
       </c>
@@ -34888,9 +35512,15 @@
       <c r="V304" t="n">
         <v>422.4</v>
       </c>
-      <c r="W304" t="inlineStr"/>
-      <c r="X304" t="inlineStr"/>
-      <c r="Y304" t="inlineStr"/>
+      <c r="W304" t="n">
+        <v>0</v>
+      </c>
+      <c r="X304" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y304" t="n">
+        <v>0</v>
+      </c>
       <c r="Z304" t="n">
         <v>0</v>
       </c>
@@ -34969,7 +35599,9 @@
       <c r="M305" t="n">
         <v>2112</v>
       </c>
-      <c r="N305" t="inlineStr"/>
+      <c r="N305" t="n">
+        <v>0</v>
+      </c>
       <c r="O305" t="n">
         <v>10</v>
       </c>
@@ -34978,7 +35610,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q305" t="inlineStr"/>
+      <c r="Q305" t="n">
+        <v>0</v>
+      </c>
       <c r="R305" t="n">
         <v>0</v>
       </c>
@@ -34994,9 +35628,15 @@
       <c r="V305" t="n">
         <v>422.4</v>
       </c>
-      <c r="W305" t="inlineStr"/>
-      <c r="X305" t="inlineStr"/>
-      <c r="Y305" t="inlineStr"/>
+      <c r="W305" t="n">
+        <v>0</v>
+      </c>
+      <c r="X305" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y305" t="n">
+        <v>0</v>
+      </c>
       <c r="Z305" t="n">
         <v>0</v>
       </c>
@@ -35075,7 +35715,9 @@
       <c r="M306" t="n">
         <v>2112</v>
       </c>
-      <c r="N306" t="inlineStr"/>
+      <c r="N306" t="n">
+        <v>0</v>
+      </c>
       <c r="O306" t="n">
         <v>10</v>
       </c>
@@ -35084,7 +35726,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q306" t="inlineStr"/>
+      <c r="Q306" t="n">
+        <v>0</v>
+      </c>
       <c r="R306" t="n">
         <v>0</v>
       </c>
@@ -35100,9 +35744,15 @@
       <c r="V306" t="n">
         <v>422.4</v>
       </c>
-      <c r="W306" t="inlineStr"/>
-      <c r="X306" t="inlineStr"/>
-      <c r="Y306" t="inlineStr"/>
+      <c r="W306" t="n">
+        <v>0</v>
+      </c>
+      <c r="X306" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y306" t="n">
+        <v>0</v>
+      </c>
       <c r="Z306" t="n">
         <v>0</v>
       </c>
@@ -35181,7 +35831,9 @@
       <c r="M307" t="n">
         <v>2112</v>
       </c>
-      <c r="N307" t="inlineStr"/>
+      <c r="N307" t="n">
+        <v>0</v>
+      </c>
       <c r="O307" t="n">
         <v>10</v>
       </c>
@@ -35190,7 +35842,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q307" t="inlineStr"/>
+      <c r="Q307" t="n">
+        <v>0</v>
+      </c>
       <c r="R307" t="n">
         <v>0</v>
       </c>
@@ -35206,9 +35860,15 @@
       <c r="V307" t="n">
         <v>422.4</v>
       </c>
-      <c r="W307" t="inlineStr"/>
-      <c r="X307" t="inlineStr"/>
-      <c r="Y307" t="inlineStr"/>
+      <c r="W307" t="n">
+        <v>0</v>
+      </c>
+      <c r="X307" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y307" t="n">
+        <v>0</v>
+      </c>
       <c r="Z307" t="n">
         <v>0</v>
       </c>
@@ -35287,7 +35947,9 @@
       <c r="M308" t="n">
         <v>34</v>
       </c>
-      <c r="N308" t="inlineStr"/>
+      <c r="N308" t="n">
+        <v>0</v>
+      </c>
       <c r="O308" t="n">
         <v>10</v>
       </c>
@@ -35296,7 +35958,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q308" t="inlineStr"/>
+      <c r="Q308" t="n">
+        <v>0</v>
+      </c>
       <c r="R308" t="n">
         <v>0</v>
       </c>
@@ -35312,9 +35976,15 @@
       <c r="V308" t="n">
         <v>13.6</v>
       </c>
-      <c r="W308" t="inlineStr"/>
-      <c r="X308" t="inlineStr"/>
-      <c r="Y308" t="inlineStr"/>
+      <c r="W308" t="n">
+        <v>0</v>
+      </c>
+      <c r="X308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y308" t="n">
+        <v>0</v>
+      </c>
       <c r="Z308" t="n">
         <v>0</v>
       </c>
@@ -35393,7 +36063,9 @@
       <c r="M309" t="n">
         <v>34</v>
       </c>
-      <c r="N309" t="inlineStr"/>
+      <c r="N309" t="n">
+        <v>0</v>
+      </c>
       <c r="O309" t="n">
         <v>10</v>
       </c>
@@ -35402,7 +36074,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q309" t="inlineStr"/>
+      <c r="Q309" t="n">
+        <v>0</v>
+      </c>
       <c r="R309" t="n">
         <v>0</v>
       </c>
@@ -35418,9 +36092,15 @@
       <c r="V309" t="n">
         <v>13.6</v>
       </c>
-      <c r="W309" t="inlineStr"/>
-      <c r="X309" t="inlineStr"/>
-      <c r="Y309" t="inlineStr"/>
+      <c r="W309" t="n">
+        <v>0</v>
+      </c>
+      <c r="X309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y309" t="n">
+        <v>0</v>
+      </c>
       <c r="Z309" t="n">
         <v>0</v>
       </c>
@@ -35499,7 +36179,9 @@
       <c r="M310" t="n">
         <v>12</v>
       </c>
-      <c r="N310" t="inlineStr"/>
+      <c r="N310" t="n">
+        <v>0</v>
+      </c>
       <c r="O310" t="n">
         <v>7</v>
       </c>
@@ -35508,7 +36190,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q310" t="inlineStr"/>
+      <c r="Q310" t="n">
+        <v>0</v>
+      </c>
       <c r="R310" t="n">
         <v>0</v>
       </c>
@@ -35524,9 +36208,15 @@
       <c r="V310" t="n">
         <v>10.28571428571428</v>
       </c>
-      <c r="W310" t="inlineStr"/>
-      <c r="X310" t="inlineStr"/>
-      <c r="Y310" t="inlineStr"/>
+      <c r="W310" t="n">
+        <v>0</v>
+      </c>
+      <c r="X310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y310" t="n">
+        <v>0</v>
+      </c>
       <c r="Z310" t="n">
         <v>0</v>
       </c>
@@ -35605,7 +36295,9 @@
       <c r="M311" t="n">
         <v>12</v>
       </c>
-      <c r="N311" t="inlineStr"/>
+      <c r="N311" t="n">
+        <v>0</v>
+      </c>
       <c r="O311" t="n">
         <v>7</v>
       </c>
@@ -35614,7 +36306,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q311" t="inlineStr"/>
+      <c r="Q311" t="n">
+        <v>0</v>
+      </c>
       <c r="R311" t="n">
         <v>0</v>
       </c>
@@ -35630,9 +36324,15 @@
       <c r="V311" t="n">
         <v>10.28571428571428</v>
       </c>
-      <c r="W311" t="inlineStr"/>
-      <c r="X311" t="inlineStr"/>
-      <c r="Y311" t="inlineStr"/>
+      <c r="W311" t="n">
+        <v>0</v>
+      </c>
+      <c r="X311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y311" t="n">
+        <v>0</v>
+      </c>
       <c r="Z311" t="n">
         <v>0</v>
       </c>
@@ -35711,7 +36411,9 @@
       <c r="M312" t="n">
         <v>56</v>
       </c>
-      <c r="N312" t="inlineStr"/>
+      <c r="N312" t="n">
+        <v>0</v>
+      </c>
       <c r="O312" t="n">
         <v>15</v>
       </c>
@@ -35720,7 +36422,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q312" t="inlineStr"/>
+      <c r="Q312" t="n">
+        <v>0</v>
+      </c>
       <c r="R312" t="n">
         <v>0</v>
       </c>
@@ -35736,9 +36440,15 @@
       <c r="V312" t="n">
         <v>7.466666666666667</v>
       </c>
-      <c r="W312" t="inlineStr"/>
-      <c r="X312" t="inlineStr"/>
-      <c r="Y312" t="inlineStr"/>
+      <c r="W312" t="n">
+        <v>0</v>
+      </c>
+      <c r="X312" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y312" t="n">
+        <v>0</v>
+      </c>
       <c r="Z312" t="n">
         <v>0</v>
       </c>
@@ -35817,7 +36527,9 @@
       <c r="M313" t="n">
         <v>56</v>
       </c>
-      <c r="N313" t="inlineStr"/>
+      <c r="N313" t="n">
+        <v>0</v>
+      </c>
       <c r="O313" t="n">
         <v>15</v>
       </c>
@@ -35826,7 +36538,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q313" t="inlineStr"/>
+      <c r="Q313" t="n">
+        <v>0</v>
+      </c>
       <c r="R313" t="n">
         <v>0</v>
       </c>
@@ -35842,9 +36556,15 @@
       <c r="V313" t="n">
         <v>7.466666666666667</v>
       </c>
-      <c r="W313" t="inlineStr"/>
-      <c r="X313" t="inlineStr"/>
-      <c r="Y313" t="inlineStr"/>
+      <c r="W313" t="n">
+        <v>0</v>
+      </c>
+      <c r="X313" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y313" t="n">
+        <v>0</v>
+      </c>
       <c r="Z313" t="n">
         <v>0</v>
       </c>
@@ -35923,7 +36643,9 @@
       <c r="M314" t="n">
         <v>56</v>
       </c>
-      <c r="N314" t="inlineStr"/>
+      <c r="N314" t="n">
+        <v>0</v>
+      </c>
       <c r="O314" t="n">
         <v>7</v>
       </c>
@@ -35932,7 +36654,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q314" t="inlineStr"/>
+      <c r="Q314" t="n">
+        <v>0</v>
+      </c>
       <c r="R314" t="n">
         <v>0</v>
       </c>
@@ -35948,9 +36672,15 @@
       <c r="V314" t="n">
         <v>16</v>
       </c>
-      <c r="W314" t="inlineStr"/>
-      <c r="X314" t="inlineStr"/>
-      <c r="Y314" t="inlineStr"/>
+      <c r="W314" t="n">
+        <v>0</v>
+      </c>
+      <c r="X314" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y314" t="n">
+        <v>0</v>
+      </c>
       <c r="Z314" t="n">
         <v>0</v>
       </c>
@@ -36029,7 +36759,9 @@
       <c r="M315" t="n">
         <v>56</v>
       </c>
-      <c r="N315" t="inlineStr"/>
+      <c r="N315" t="n">
+        <v>0</v>
+      </c>
       <c r="O315" t="n">
         <v>7</v>
       </c>
@@ -36038,7 +36770,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q315" t="inlineStr"/>
+      <c r="Q315" t="n">
+        <v>0</v>
+      </c>
       <c r="R315" t="n">
         <v>0</v>
       </c>
@@ -36054,9 +36788,15 @@
       <c r="V315" t="n">
         <v>16</v>
       </c>
-      <c r="W315" t="inlineStr"/>
-      <c r="X315" t="inlineStr"/>
-      <c r="Y315" t="inlineStr"/>
+      <c r="W315" t="n">
+        <v>0</v>
+      </c>
+      <c r="X315" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y315" t="n">
+        <v>0</v>
+      </c>
       <c r="Z315" t="n">
         <v>0</v>
       </c>
@@ -36135,7 +36875,9 @@
       <c r="M316" t="n">
         <v>6</v>
       </c>
-      <c r="N316" t="inlineStr"/>
+      <c r="N316" t="n">
+        <v>0</v>
+      </c>
       <c r="O316" t="n">
         <v>15</v>
       </c>
@@ -36144,7 +36886,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q316" t="inlineStr"/>
+      <c r="Q316" t="n">
+        <v>0</v>
+      </c>
       <c r="R316" t="n">
         <v>0</v>
       </c>
@@ -36160,9 +36904,15 @@
       <c r="V316" t="n">
         <v>0.8</v>
       </c>
-      <c r="W316" t="inlineStr"/>
-      <c r="X316" t="inlineStr"/>
-      <c r="Y316" t="inlineStr"/>
+      <c r="W316" t="n">
+        <v>0</v>
+      </c>
+      <c r="X316" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y316" t="n">
+        <v>0</v>
+      </c>
       <c r="Z316" t="n">
         <v>0</v>
       </c>
@@ -36241,7 +36991,9 @@
       <c r="M317" t="n">
         <v>6</v>
       </c>
-      <c r="N317" t="inlineStr"/>
+      <c r="N317" t="n">
+        <v>0</v>
+      </c>
       <c r="O317" t="n">
         <v>15</v>
       </c>
@@ -36250,7 +37002,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q317" t="inlineStr"/>
+      <c r="Q317" t="n">
+        <v>0</v>
+      </c>
       <c r="R317" t="n">
         <v>0</v>
       </c>
@@ -36266,9 +37020,15 @@
       <c r="V317" t="n">
         <v>0.8</v>
       </c>
-      <c r="W317" t="inlineStr"/>
-      <c r="X317" t="inlineStr"/>
-      <c r="Y317" t="inlineStr"/>
+      <c r="W317" t="n">
+        <v>0</v>
+      </c>
+      <c r="X317" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y317" t="n">
+        <v>0</v>
+      </c>
       <c r="Z317" t="n">
         <v>0</v>
       </c>
@@ -36347,7 +37107,9 @@
       <c r="M318" t="n">
         <v>6</v>
       </c>
-      <c r="N318" t="inlineStr"/>
+      <c r="N318" t="n">
+        <v>0</v>
+      </c>
       <c r="O318" t="n">
         <v>15</v>
       </c>
@@ -36356,7 +37118,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q318" t="inlineStr"/>
+      <c r="Q318" t="n">
+        <v>0</v>
+      </c>
       <c r="R318" t="n">
         <v>0</v>
       </c>
@@ -36372,9 +37136,15 @@
       <c r="V318" t="n">
         <v>0.8</v>
       </c>
-      <c r="W318" t="inlineStr"/>
-      <c r="X318" t="inlineStr"/>
-      <c r="Y318" t="inlineStr"/>
+      <c r="W318" t="n">
+        <v>0</v>
+      </c>
+      <c r="X318" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y318" t="n">
+        <v>0</v>
+      </c>
       <c r="Z318" t="n">
         <v>0</v>
       </c>
@@ -36453,7 +37223,9 @@
       <c r="M319" t="n">
         <v>6</v>
       </c>
-      <c r="N319" t="inlineStr"/>
+      <c r="N319" t="n">
+        <v>0</v>
+      </c>
       <c r="O319" t="n">
         <v>5</v>
       </c>
@@ -36462,7 +37234,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q319" t="inlineStr"/>
+      <c r="Q319" t="n">
+        <v>0</v>
+      </c>
       <c r="R319" t="n">
         <v>0</v>
       </c>
@@ -36478,9 +37252,15 @@
       <c r="V319" t="n">
         <v>3.600000000000001</v>
       </c>
-      <c r="W319" t="inlineStr"/>
-      <c r="X319" t="inlineStr"/>
-      <c r="Y319" t="inlineStr"/>
+      <c r="W319" t="n">
+        <v>0</v>
+      </c>
+      <c r="X319" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y319" t="n">
+        <v>0</v>
+      </c>
       <c r="Z319" t="n">
         <v>0</v>
       </c>
@@ -36559,7 +37339,9 @@
       <c r="M320" t="n">
         <v>6</v>
       </c>
-      <c r="N320" t="inlineStr"/>
+      <c r="N320" t="n">
+        <v>0</v>
+      </c>
       <c r="O320" t="n">
         <v>5</v>
       </c>
@@ -36568,7 +37350,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q320" t="inlineStr"/>
+      <c r="Q320" t="n">
+        <v>0</v>
+      </c>
       <c r="R320" t="n">
         <v>0</v>
       </c>
@@ -36584,9 +37368,15 @@
       <c r="V320" t="n">
         <v>3.600000000000001</v>
       </c>
-      <c r="W320" t="inlineStr"/>
-      <c r="X320" t="inlineStr"/>
-      <c r="Y320" t="inlineStr"/>
+      <c r="W320" t="n">
+        <v>0</v>
+      </c>
+      <c r="X320" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y320" t="n">
+        <v>0</v>
+      </c>
       <c r="Z320" t="n">
         <v>0</v>
       </c>
@@ -36665,7 +37455,9 @@
       <c r="M321" t="n">
         <v>12</v>
       </c>
-      <c r="N321" t="inlineStr"/>
+      <c r="N321" t="n">
+        <v>0</v>
+      </c>
       <c r="O321" t="n">
         <v>5</v>
       </c>
@@ -36674,7 +37466,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q321" t="inlineStr"/>
+      <c r="Q321" t="n">
+        <v>0</v>
+      </c>
       <c r="R321" t="n">
         <v>0</v>
       </c>
@@ -36690,9 +37484,15 @@
       <c r="V321" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W321" t="inlineStr"/>
-      <c r="X321" t="inlineStr"/>
-      <c r="Y321" t="inlineStr"/>
+      <c r="W321" t="n">
+        <v>0</v>
+      </c>
+      <c r="X321" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y321" t="n">
+        <v>0</v>
+      </c>
       <c r="Z321" t="n">
         <v>0</v>
       </c>
@@ -36771,7 +37571,9 @@
       <c r="M322" t="n">
         <v>12</v>
       </c>
-      <c r="N322" t="inlineStr"/>
+      <c r="N322" t="n">
+        <v>0</v>
+      </c>
       <c r="O322" t="n">
         <v>5</v>
       </c>
@@ -36780,7 +37582,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q322" t="inlineStr"/>
+      <c r="Q322" t="n">
+        <v>0</v>
+      </c>
       <c r="R322" t="n">
         <v>0</v>
       </c>
@@ -36796,9 +37600,15 @@
       <c r="V322" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W322" t="inlineStr"/>
-      <c r="X322" t="inlineStr"/>
-      <c r="Y322" t="inlineStr"/>
+      <c r="W322" t="n">
+        <v>0</v>
+      </c>
+      <c r="X322" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y322" t="n">
+        <v>0</v>
+      </c>
       <c r="Z322" t="n">
         <v>0</v>
       </c>
@@ -36877,7 +37687,9 @@
       <c r="M323" t="n">
         <v>12</v>
       </c>
-      <c r="N323" t="inlineStr"/>
+      <c r="N323" t="n">
+        <v>0</v>
+      </c>
       <c r="O323" t="n">
         <v>5</v>
       </c>
@@ -36886,7 +37698,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q323" t="inlineStr"/>
+      <c r="Q323" t="n">
+        <v>0</v>
+      </c>
       <c r="R323" t="n">
         <v>0</v>
       </c>
@@ -36902,9 +37716,15 @@
       <c r="V323" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W323" t="inlineStr"/>
-      <c r="X323" t="inlineStr"/>
-      <c r="Y323" t="inlineStr"/>
+      <c r="W323" t="n">
+        <v>0</v>
+      </c>
+      <c r="X323" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y323" t="n">
+        <v>0</v>
+      </c>
       <c r="Z323" t="n">
         <v>0</v>
       </c>
@@ -36983,7 +37803,9 @@
       <c r="M324" t="n">
         <v>12</v>
       </c>
-      <c r="N324" t="inlineStr"/>
+      <c r="N324" t="n">
+        <v>0</v>
+      </c>
       <c r="O324" t="n">
         <v>5</v>
       </c>
@@ -36992,7 +37814,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q324" t="inlineStr"/>
+      <c r="Q324" t="n">
+        <v>0</v>
+      </c>
       <c r="R324" t="n">
         <v>0</v>
       </c>
@@ -37008,9 +37832,15 @@
       <c r="V324" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W324" t="inlineStr"/>
-      <c r="X324" t="inlineStr"/>
-      <c r="Y324" t="inlineStr"/>
+      <c r="W324" t="n">
+        <v>0</v>
+      </c>
+      <c r="X324" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y324" t="n">
+        <v>0</v>
+      </c>
       <c r="Z324" t="n">
         <v>0</v>
       </c>
@@ -37089,7 +37919,9 @@
       <c r="M325" t="n">
         <v>12</v>
       </c>
-      <c r="N325" t="inlineStr"/>
+      <c r="N325" t="n">
+        <v>0</v>
+      </c>
       <c r="O325" t="n">
         <v>5</v>
       </c>
@@ -37098,7 +37930,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q325" t="inlineStr"/>
+      <c r="Q325" t="n">
+        <v>0</v>
+      </c>
       <c r="R325" t="n">
         <v>0</v>
       </c>
@@ -37114,9 +37948,15 @@
       <c r="V325" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W325" t="inlineStr"/>
-      <c r="X325" t="inlineStr"/>
-      <c r="Y325" t="inlineStr"/>
+      <c r="W325" t="n">
+        <v>0</v>
+      </c>
+      <c r="X325" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y325" t="n">
+        <v>0</v>
+      </c>
       <c r="Z325" t="n">
         <v>0</v>
       </c>
@@ -37195,7 +38035,9 @@
       <c r="M326" t="n">
         <v>12</v>
       </c>
-      <c r="N326" t="inlineStr"/>
+      <c r="N326" t="n">
+        <v>0</v>
+      </c>
       <c r="O326" t="n">
         <v>5</v>
       </c>
@@ -37204,7 +38046,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q326" t="inlineStr"/>
+      <c r="Q326" t="n">
+        <v>0</v>
+      </c>
       <c r="R326" t="n">
         <v>0</v>
       </c>
@@ -37220,9 +38064,15 @@
       <c r="V326" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W326" t="inlineStr"/>
-      <c r="X326" t="inlineStr"/>
-      <c r="Y326" t="inlineStr"/>
+      <c r="W326" t="n">
+        <v>0</v>
+      </c>
+      <c r="X326" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y326" t="n">
+        <v>0</v>
+      </c>
       <c r="Z326" t="n">
         <v>0</v>
       </c>
@@ -37301,7 +38151,9 @@
       <c r="M327" t="n">
         <v>12</v>
       </c>
-      <c r="N327" t="inlineStr"/>
+      <c r="N327" t="n">
+        <v>0</v>
+      </c>
       <c r="O327" t="n">
         <v>5</v>
       </c>
@@ -37310,7 +38162,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q327" t="inlineStr"/>
+      <c r="Q327" t="n">
+        <v>0</v>
+      </c>
       <c r="R327" t="n">
         <v>0</v>
       </c>
@@ -37326,9 +38180,15 @@
       <c r="V327" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W327" t="inlineStr"/>
-      <c r="X327" t="inlineStr"/>
-      <c r="Y327" t="inlineStr"/>
+      <c r="W327" t="n">
+        <v>0</v>
+      </c>
+      <c r="X327" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y327" t="n">
+        <v>0</v>
+      </c>
       <c r="Z327" t="n">
         <v>0</v>
       </c>
@@ -37407,7 +38267,9 @@
       <c r="M328" t="n">
         <v>12</v>
       </c>
-      <c r="N328" t="inlineStr"/>
+      <c r="N328" t="n">
+        <v>0</v>
+      </c>
       <c r="O328" t="n">
         <v>5</v>
       </c>
@@ -37416,7 +38278,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q328" t="inlineStr"/>
+      <c r="Q328" t="n">
+        <v>0</v>
+      </c>
       <c r="R328" t="n">
         <v>0</v>
       </c>
@@ -37432,9 +38296,15 @@
       <c r="V328" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W328" t="inlineStr"/>
-      <c r="X328" t="inlineStr"/>
-      <c r="Y328" t="inlineStr"/>
+      <c r="W328" t="n">
+        <v>0</v>
+      </c>
+      <c r="X328" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y328" t="n">
+        <v>0</v>
+      </c>
       <c r="Z328" t="n">
         <v>0</v>
       </c>
@@ -37513,7 +38383,9 @@
       <c r="M329" t="n">
         <v>12</v>
       </c>
-      <c r="N329" t="inlineStr"/>
+      <c r="N329" t="n">
+        <v>0</v>
+      </c>
       <c r="O329" t="n">
         <v>5</v>
       </c>
@@ -37522,7 +38394,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q329" t="inlineStr"/>
+      <c r="Q329" t="n">
+        <v>0</v>
+      </c>
       <c r="R329" t="n">
         <v>0</v>
       </c>
@@ -37538,9 +38412,15 @@
       <c r="V329" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W329" t="inlineStr"/>
-      <c r="X329" t="inlineStr"/>
-      <c r="Y329" t="inlineStr"/>
+      <c r="W329" t="n">
+        <v>0</v>
+      </c>
+      <c r="X329" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y329" t="n">
+        <v>0</v>
+      </c>
       <c r="Z329" t="n">
         <v>0</v>
       </c>
@@ -37619,7 +38499,9 @@
       <c r="M330" t="n">
         <v>12</v>
       </c>
-      <c r="N330" t="inlineStr"/>
+      <c r="N330" t="n">
+        <v>0</v>
+      </c>
       <c r="O330" t="n">
         <v>5</v>
       </c>
@@ -37628,7 +38510,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q330" t="inlineStr"/>
+      <c r="Q330" t="n">
+        <v>0</v>
+      </c>
       <c r="R330" t="n">
         <v>0</v>
       </c>
@@ -37644,9 +38528,15 @@
       <c r="V330" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W330" t="inlineStr"/>
-      <c r="X330" t="inlineStr"/>
-      <c r="Y330" t="inlineStr"/>
+      <c r="W330" t="n">
+        <v>0</v>
+      </c>
+      <c r="X330" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y330" t="n">
+        <v>0</v>
+      </c>
       <c r="Z330" t="n">
         <v>0</v>
       </c>
@@ -37725,7 +38615,9 @@
       <c r="M331" t="n">
         <v>12</v>
       </c>
-      <c r="N331" t="inlineStr"/>
+      <c r="N331" t="n">
+        <v>0</v>
+      </c>
       <c r="O331" t="n">
         <v>5</v>
       </c>
@@ -37734,7 +38626,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q331" t="inlineStr"/>
+      <c r="Q331" t="n">
+        <v>0</v>
+      </c>
       <c r="R331" t="n">
         <v>0</v>
       </c>
@@ -37750,9 +38644,15 @@
       <c r="V331" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W331" t="inlineStr"/>
-      <c r="X331" t="inlineStr"/>
-      <c r="Y331" t="inlineStr"/>
+      <c r="W331" t="n">
+        <v>0</v>
+      </c>
+      <c r="X331" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y331" t="n">
+        <v>0</v>
+      </c>
       <c r="Z331" t="n">
         <v>0</v>
       </c>
@@ -37831,7 +38731,9 @@
       <c r="M332" t="n">
         <v>12</v>
       </c>
-      <c r="N332" t="inlineStr"/>
+      <c r="N332" t="n">
+        <v>0</v>
+      </c>
       <c r="O332" t="n">
         <v>5</v>
       </c>
@@ -37840,7 +38742,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q332" t="inlineStr"/>
+      <c r="Q332" t="n">
+        <v>0</v>
+      </c>
       <c r="R332" t="n">
         <v>0</v>
       </c>
@@ -37856,9 +38760,15 @@
       <c r="V332" t="n">
         <v>4.800000000000001</v>
       </c>
-      <c r="W332" t="inlineStr"/>
-      <c r="X332" t="inlineStr"/>
-      <c r="Y332" t="inlineStr"/>
+      <c r="W332" t="n">
+        <v>0</v>
+      </c>
+      <c r="X332" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y332" t="n">
+        <v>0</v>
+      </c>
       <c r="Z332" t="n">
         <v>0</v>
       </c>
@@ -37937,7 +38847,9 @@
       <c r="M333" t="n">
         <v>56</v>
       </c>
-      <c r="N333" t="inlineStr"/>
+      <c r="N333" t="n">
+        <v>0</v>
+      </c>
       <c r="O333" t="n">
         <v>7</v>
       </c>
@@ -37946,7 +38858,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q333" t="inlineStr"/>
+      <c r="Q333" t="n">
+        <v>0</v>
+      </c>
       <c r="R333" t="n">
         <v>0</v>
       </c>
@@ -37962,9 +38876,15 @@
       <c r="V333" t="n">
         <v>40</v>
       </c>
-      <c r="W333" t="inlineStr"/>
-      <c r="X333" t="inlineStr"/>
-      <c r="Y333" t="inlineStr"/>
+      <c r="W333" t="n">
+        <v>0</v>
+      </c>
+      <c r="X333" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y333" t="n">
+        <v>0</v>
+      </c>
       <c r="Z333" t="n">
         <v>0</v>
       </c>
@@ -38043,7 +38963,9 @@
       <c r="M334" t="n">
         <v>20</v>
       </c>
-      <c r="N334" t="inlineStr"/>
+      <c r="N334" t="n">
+        <v>0</v>
+      </c>
       <c r="O334" t="n">
         <v>7</v>
       </c>
@@ -38052,7 +38974,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="Q334" t="inlineStr"/>
+      <c r="Q334" t="n">
+        <v>0</v>
+      </c>
       <c r="R334" t="n">
         <v>0</v>
       </c>
@@ -38068,9 +38992,15 @@
       <c r="V334" t="n">
         <v>11.42857142857143</v>
       </c>
-      <c r="W334" t="inlineStr"/>
-      <c r="X334" t="inlineStr"/>
-      <c r="Y334" t="inlineStr"/>
+      <c r="W334" t="n">
+        <v>0</v>
+      </c>
+      <c r="X334" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y334" t="n">
+        <v>0</v>
+      </c>
       <c r="Z334" t="n">
         <v>0</v>
       </c>

</xml_diff>